<commit_message>
Added react-redux - store, first reducer, subscribe
</commit_message>
<xml_diff>
--- a/список ароматизаторов.xlsx
+++ b/список ароматизаторов.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="412">
   <si>
     <t>A</t>
   </si>
@@ -6132,6 +6132,18 @@
   </si>
   <si>
     <t>Wintergreen (Мятные кофеты)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id: </t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name: </t>
+  </si>
+  <si>
+    <t>isSelected: false },</t>
   </si>
 </sst>
 </file>
@@ -8285,10 +8297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B197"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="M168" sqref="M168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8296,7 +8308,7 @@
     <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>220</v>
       </c>
@@ -8304,8 +8316,24 @@
         <f>CONCATENATE("'",A1,"', ")</f>
         <v xml:space="preserve">'Absinthe (Абсент)', </v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="F1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1" t="s">
+        <v>411</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE($F$1,$G$1,B1,$H$1,B1,$I$1)</f>
+        <v>{id: 'Absinthe (Абсент)', name: 'Absinthe (Абсент)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -8313,8 +8341,12 @@
         <f t="shared" ref="B2:B65" si="0">CONCATENATE("'",A2,"', ")</f>
         <v xml:space="preserve">'Acai (Ягода асаи)', </v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K65" si="1">CONCATENATE($F$1,$G$1,B2,$H$1,B2,$I$1)</f>
+        <v>{id: 'Acai (Ягода асаи)', name: 'Acai (Ягода асаи)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -8322,8 +8354,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Acetyl Pyrazine (Ацетил пиразин)', </v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="K3" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Acetyl Pyrazine (Ацетил пиразин)', name: 'Acetyl Pyrazine (Ацетил пиразин)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -8331,8 +8367,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Almond (Миндаль)', </v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Almond (Миндаль)', name: 'Almond (Миндаль)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -8340,8 +8380,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Apple (Яблоко)', </v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Apple (Яблоко)', name: 'Apple (Яблоко)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -8349,8 +8393,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Apple (tart granny smith) (Яблоко (Гренни Смит))', </v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Apple (tart granny smith) (Яблоко (Гренни Смит))', name: 'Apple (tart granny smith) (Яблоко (Гренни Смит))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -8358,8 +8406,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Apple Candy (Яблочный мармелад)', </v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Apple Candy (Яблочный мармелад)', name: 'Apple Candy (Яблочный мармелад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>227</v>
       </c>
@@ -8367,8 +8419,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Apple Pie (Яблочный пирог)', </v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Apple Pie (Яблочный пирог)', name: 'Apple Pie (Яблочный пирог)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>228</v>
       </c>
@@ -8376,8 +8432,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Apricot (Абрикос)', </v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Apricot (Абрикос)', name: 'Apricot (Абрикос)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>229</v>
       </c>
@@ -8385,8 +8445,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Banana (Банан)', </v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Banana (Банан)', name: 'Banana (Банан)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>230</v>
       </c>
@@ -8394,8 +8458,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Banana Cream (Банановый крем)', </v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Banana Cream (Банановый крем)', name: 'Banana Cream (Банановый крем)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>231</v>
       </c>
@@ -8403,8 +8471,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Banana Nut Bread (Банановый хлеб)', </v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Banana Nut Bread (Банановый хлеб)', name: 'Banana Nut Bread (Банановый хлеб)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>232</v>
       </c>
@@ -8412,8 +8484,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bananas Foster (Банановый фостер)', </v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bananas Foster (Банановый фостер)', name: 'Bananas Foster (Банановый фостер)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>233</v>
       </c>
@@ -8421,8 +8497,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bavarian Cream (Баварский крем)', </v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bavarian Cream (Баварский крем)', name: 'Bavarian Cream (Баварский крем)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -8430,8 +8510,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Berry Crunch (Ягодные хлопья)', </v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Berry Crunch (Ягодные хлопья)', name: 'Berry Crunch (Ягодные хлопья)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>235</v>
       </c>
@@ -8439,8 +8523,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bitter Nut Extra (Горький орех)', </v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bitter Nut Extra (Горький орех)', name: 'Bitter Nut Extra (Горький орех)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -8448,8 +8536,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bittersweet Chocolate (Биттерсвит шоколад)', </v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bittersweet Chocolate (Биттерсвит шоколад)', name: 'Bittersweet Chocolate (Биттерсвит шоколад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>237</v>
       </c>
@@ -8457,8 +8549,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Black Cherry (Черешня)', </v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Black Cherry (Черешня)', name: 'Black Cherry (Черешня)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>238</v>
       </c>
@@ -8466,8 +8562,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Black Currant (Черная смородина)', </v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Black Currant (Черная смородина)', name: 'Black Currant (Черная смородина)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>239</v>
       </c>
@@ -8475,8 +8575,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Black Honey (Черный мед и табак)', </v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Black Honey (Черный мед и табак)', name: 'Black Honey (Черный мед и табак)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -8484,8 +8588,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Black Tea (Черный чай)', </v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Black Tea (Черный чай)', name: 'Black Tea (Черный чай)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>240</v>
       </c>
@@ -8493,8 +8601,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Blackberry (Ежевика)', </v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Blackberry (Ежевика)', name: 'Blackberry (Ежевика)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>241</v>
       </c>
@@ -8502,8 +8614,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Blue Raspberry (Голубая малина)', </v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Blue Raspberry (Голубая малина)', name: 'Blue Raspberry (Голубая малина)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>242</v>
       </c>
@@ -8511,8 +8627,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Blueberry (Extra) (Черника)', </v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Blueberry (Extra) (Черника)', name: 'Blueberry (Extra) (Черника)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>243</v>
       </c>
@@ -8520,8 +8640,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Blueberry Candy (Черничные леденцы)', </v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Blueberry Candy (Черничные леденцы)', name: 'Blueberry Candy (Черничные леденцы)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>244</v>
       </c>
@@ -8529,8 +8653,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Blueberry Wild (Дикая черника)', </v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Blueberry Wild (Дикая черника)', name: 'Blueberry Wild (Дикая черника)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -8538,8 +8666,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Boysenberry (Шелковица )', </v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Boysenberry (Шелковица )', name: 'Boysenberry (Шелковица )', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -8547,8 +8679,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Brandy (Бренди)', </v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Brandy (Бренди)', name: 'Brandy (Бренди)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -8556,8 +8692,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Brown Sugar (Коричневый сахар)', </v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Brown Sugar (Коричневый сахар)', name: 'Brown Sugar (Коричневый сахар)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -8565,8 +8705,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bubblegum (Жвачка)', </v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bubblegum (Жвачка)', name: 'Bubblegum (Жвачка)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>248</v>
       </c>
@@ -8574,8 +8718,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Bubblegum (Fruity) (Жвачка (Фруктовая))', </v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Bubblegum (Fruity) (Жвачка (Фруктовая))', name: 'Bubblegum (Fruity) (Жвачка (Фруктовая))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>249</v>
       </c>
@@ -8583,8 +8731,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Butter (Масло)', </v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Butter (Масло)', name: 'Butter (Масло)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>250</v>
       </c>
@@ -8592,8 +8744,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Butterscotch (Ирис)', </v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Butterscotch (Ирис)', name: 'Butterscotch (Ирис)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>251</v>
       </c>
@@ -8601,8 +8757,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cantaloupe (Канталупа)', </v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cantaloupe (Канталупа)', name: 'Cantaloupe (Канталупа)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>252</v>
       </c>
@@ -8610,8 +8770,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cappucсino (Каппучино)', </v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cappucсino (Каппучино)', name: 'Cappucсino (Каппучино)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>253</v>
       </c>
@@ -8619,8 +8783,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Caramel (Карамель)', </v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Caramel (Карамель)', name: 'Caramel (Карамель)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>254</v>
       </c>
@@ -8628,8 +8796,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Caramel (Original) (Карамель (Оригинальная))', </v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Caramel (Original) (Карамель (Оригинальная))', name: 'Caramel (Original) (Карамель (Оригинальная))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -8637,8 +8809,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Caramel Candy (Карамельная конфета)', </v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Caramel Candy (Карамельная конфета)', name: 'Caramel Candy (Карамельная конфета)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>256</v>
       </c>
@@ -8646,8 +8822,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Caramel Cappuccino (Карамель-каппучино)', </v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Caramel Cappuccino (Карамель-каппучино)', name: 'Caramel Cappuccino (Карамель-каппучино)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>257</v>
       </c>
@@ -8655,8 +8835,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Chai Tea (Чай)', </v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Chai Tea (Чай)', name: 'Chai Tea (Чай)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>258</v>
       </c>
@@ -8664,8 +8848,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Champagne (Шампанское)', </v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Champagne (Шампанское)', name: 'Champagne (Шампанское)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>259</v>
       </c>
@@ -8673,8 +8861,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cheesecake (Чизкейк)', </v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cheesecake (Чизкейк)', name: 'Cheesecake (Чизкейк)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>260</v>
       </c>
@@ -8682,8 +8874,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cheesecake (Graham Crust) (Чизкейк (корочка))', </v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cheesecake (Graham Crust) (Чизкейк (корочка))', name: 'Cheesecake (Graham Crust) (Чизкейк (корочка))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>261</v>
       </c>
@@ -8691,8 +8887,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cherry Blossom (Цветущая вишня)', </v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cherry Blossom (Цветущая вишня)', name: 'Cherry Blossom (Цветущая вишня)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>262</v>
       </c>
@@ -8700,8 +8900,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cherry Extract (Экстракт вишни)', </v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cherry Extract (Экстракт вишни)', name: 'Cherry Extract (Экстракт вишни)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -8709,8 +8913,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Chocolate (Шоколад)', </v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Chocolate (Шоколад)', name: 'Chocolate (Шоколад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>263</v>
       </c>
@@ -8718,8 +8926,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cinnamon (Корица)', </v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cinnamon (Корица)', name: 'Cinnamon (Корица)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>264</v>
       </c>
@@ -8727,8 +8939,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cinnamon Danish (Корица датская)', </v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cinnamon Danish (Корица датская)', name: 'Cinnamon Danish (Корица датская)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>265</v>
       </c>
@@ -8736,8 +8952,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cinnamon Red Hot (Корица)', </v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cinnamon Red Hot (Корица)', name: 'Cinnamon Red Hot (Корица)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>266</v>
       </c>
@@ -8745,8 +8965,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cinnamon Spice (Острая корица)', </v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="K50" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cinnamon Spice (Острая корица)', name: 'Cinnamon Spice (Острая корица)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>267</v>
       </c>
@@ -8754,8 +8978,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cinnamon Sugar Cookie (Печенье с корицей)', </v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cinnamon Sugar Cookie (Печенье с корицей)', name: 'Cinnamon Sugar Cookie (Печенье с корицей)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>268</v>
       </c>
@@ -8763,8 +8991,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Citrus Punch (Цитрусовый пунш)', </v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Citrus Punch (Цитрусовый пунш)', name: 'Citrus Punch (Цитрусовый пунш)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>269</v>
       </c>
@@ -8772,8 +9004,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Clove (Гвоздика)', </v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="K53" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Clove (Гвоздика)', name: 'Clove (Гвоздика)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>270</v>
       </c>
@@ -8781,8 +9017,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cocoa Rounds (Шоколадные шарики)', </v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="K54" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cocoa Rounds (Шоколадные шарики)', name: 'Cocoa Rounds (Шоколадные шарики)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>271</v>
       </c>
@@ -8790,8 +9030,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Coconut (Кокос)', </v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="K55" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Coconut (Кокос)', name: 'Coconut (Кокос)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>272</v>
       </c>
@@ -8799,8 +9043,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Coconut (Extra) (Кокос (Экстра))', </v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="K56" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Coconut (Extra) (Кокос (Экстра))', name: 'Coconut (Extra) (Кокос (Экстра))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>273</v>
       </c>
@@ -8808,8 +9056,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Coconut Candy (Кокосовые конфеты)', </v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="K57" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Coconut Candy (Кокосовые конфеты)', name: 'Coconut Candy (Кокосовые конфеты)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>274</v>
       </c>
@@ -8817,8 +9069,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Coffee (Кофе)', </v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="K58" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Coffee (Кофе)', name: 'Coffee (Кофе)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>275</v>
       </c>
@@ -8826,8 +9082,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cotton Candy (Сладкая вата)', </v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="K59" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cotton Candy (Сладкая вата)', name: 'Cotton Candy (Сладкая вата)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -8835,8 +9095,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cranberry (Клюква)', </v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="K60" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cranberry (Клюква)', name: 'Cranberry (Клюква)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>277</v>
       </c>
@@ -8844,8 +9108,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cream Soda (Крем-сода)', </v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="K61" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cream Soda (Крем-сода)', name: 'Cream Soda (Крем-сода)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>278</v>
       </c>
@@ -8853,8 +9121,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Creme de Menthe (Сладкий мятный ликер)', </v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="K62" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Creme de Menthe (Сладкий мятный ликер)', name: 'Creme de Menthe (Сладкий мятный ликер)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>279</v>
       </c>
@@ -8862,8 +9134,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Cucumber (Огурец)', </v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="K63" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Cucumber (Огурец)', name: 'Cucumber (Огурец)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>280</v>
       </c>
@@ -8871,8 +9147,12 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'Dairy/Milk (Молоко)', </v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="K64" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'Dairy/Milk (Молоко)', name: 'Dairy/Milk (Молоко)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -8880,1193 +9160,1725 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">'DK Tobacco Base (Табак)', </v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="K65" t="str">
+        <f t="shared" si="1"/>
+        <v>{id: 'DK Tobacco Base (Табак)', name: 'DK Tobacco Base (Табак)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>282</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B129" si="1">CONCATENATE("'",A66,"', ")</f>
+        <f t="shared" ref="B66:B129" si="2">CONCATENATE("'",A66,"', ")</f>
         <v xml:space="preserve">'Double Chocolate (Clear) (Двойной шоколад)', </v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="K66" t="str">
+        <f t="shared" ref="K66:K129" si="3">CONCATENATE($F$1,$G$1,B66,$H$1,B66,$I$1)</f>
+        <v>{id: 'Double Chocolate (Clear) (Двойной шоколад)', name: 'Double Chocolate (Clear) (Двойной шоколад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>283</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Double Chocolate (Dark) (Двойной шоколад (Темный))', </v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="K67" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Double Chocolate (Dark) (Двойной шоколад (Темный))', name: 'Double Chocolate (Dark) (Двойной шоколад (Темный))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" t="s">
         <v>284</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Dragonfruit (Драгонфрут (питайя))', </v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="K68" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Dragonfruit (Драгонфрут (питайя))', name: 'Dragonfruit (Драгонфрут (питайя))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>285</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Dulce de Leche (Сгущенное молоко)', </v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="K69" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Dulce de Leche (Сгущенное молоко)', name: 'Dulce de Leche (Сгущенное молоко)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>286</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Earl Grey Tea (Эрл-грей)', </v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="K70" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Earl Grey Tea (Эрл-грей)', name: 'Earl Grey Tea (Эрл-грей)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>287</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Elderberry (Бузина)', </v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="K71" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Elderberry (Бузина)', name: 'Elderberry (Бузина)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>288</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Energy Drink (Энергетический напиток)', </v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="K72" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Energy Drink (Энергетический напиток)', name: 'Energy Drink (Энергетический напиток)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>289</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'English Toffee (Тоффи)', </v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="K73" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'English Toffee (Тоффи)', name: 'English Toffee (Тоффи)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>290</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Espresso (Эспрессо)', </v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="K74" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Espresso (Эспрессо)', name: 'Espresso (Эспрессо)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>291</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Ethyl Maltol (Этил мальтол)', </v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="K75" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Ethyl Maltol (Этил мальтол)', name: 'Ethyl Maltol (Этил мальтол)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>292</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'French Vanilla (Французкая ваниль)', </v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="K76" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'French Vanilla (Французкая ваниль)', name: 'French Vanilla (Французкая ваниль)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>82</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'French Vanilla Deluxe (Французкая ваниль (Делюкс))', </v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="K77" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'French Vanilla Deluxe (Французкая ваниль (Делюкс))', name: 'French Vanilla Deluxe (Французкая ваниль (Делюкс))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>293</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Frosted Donut (Пончик)', </v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="K78" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Frosted Donut (Пончик)', name: 'Frosted Donut (Пончик)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>294</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Fruit Circles (Фруктовые кольца)', </v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="K79" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Fruit Circles (Фруктовые кольца)', name: 'Fruit Circles (Фруктовые кольца)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>295</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Fruit Circles With Milk (Фруктовые кольца с молоком)', </v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="K80" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Fruit Circles With Milk (Фруктовые кольца с молоком)', name: 'Fruit Circles With Milk (Фруктовые кольца с молоком)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>296</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Fruity Stick Gum (Жвачка (Fruity Stick))', </v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="K81" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Fruity Stick Gum (Жвачка (Fruity Stick))', name: 'Fruity Stick Gum (Жвачка (Fruity Stick))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>297</v>
       </c>
       <c r="B82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Fudge Brownie (Брауни)', </v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="K82" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Fudge Brownie (Брауни)', name: 'Fudge Brownie (Брауни)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>298</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Ginger Ale (Имбирный Эль)', </v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="K83" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Ginger Ale (Имбирный Эль)', name: 'Ginger Ale (Имбирный Эль)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>299</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Gingerbread (Имбирный пряник)', </v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="K84" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Gingerbread (Имбирный пряник)', name: 'Gingerbread (Имбирный пряник)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>300</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Graham Cracker (Грэхем крекер)', </v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="K85" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Graham Cracker (Грэхем крекер)', name: 'Graham Cracker (Грэхем крекер)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>301</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Graham Cracker Clear (Грэхем крекер)', </v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="K86" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Graham Cracker Clear (Грэхем крекер)', name: 'Graham Cracker Clear (Грэхем крекер)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>302</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Grape Candy (Виноградные леденцы)', </v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="K87" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Grape Candy (Виноградные леденцы)', name: 'Grape Candy (Виноградные леденцы)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>303</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Grape Juice (Виноградный сок)', </v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="K88" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Grape Juice (Виноградный сок)', name: 'Grape Juice (Виноградный сок)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>304</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Greek Yogurt (Греческий йогурт)', </v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="K89" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Greek Yogurt (Греческий йогурт)', name: 'Greek Yogurt (Греческий йогурт)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>305</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Green Apple (Зеленое яблоко)', </v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="K90" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Green Apple (Зеленое яблоко)', name: 'Green Apple (Зеленое яблоко)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>306</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Green Tea (Зеленый чай)', </v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="K91" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Green Tea (Зеленый чай)', name: 'Green Tea (Зеленый чай)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>307</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Guava (Гуайява)', </v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="K92" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Guava (Гуайява)', name: 'Guava (Гуайява)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>308</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Gummy Candy (Тянучки)', </v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="K93" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Gummy Candy (Тянучки)', name: 'Gummy Candy (Тянучки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>309</v>
       </c>
       <c r="B94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Hazelnut (Лесной орех)', </v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="K94" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Hazelnut (Лесной орех)', name: 'Hazelnut (Лесной орех)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>310</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Hibiscus (Гибискус)', </v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="K95" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Hibiscus (Гибискус)', name: 'Hibiscus (Гибискус)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>311</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Honey (Мед)', </v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="K96" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Honey (Мед)', name: 'Honey (Мед)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>312</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Honeydew (Медовая дыня)', </v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="K97" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Honeydew (Медовая дыня)', name: 'Honeydew (Медовая дыня)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>313</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Honeydew II (Медовая дыня (версия 2))', </v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="K98" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Honeydew II (Медовая дыня (версия 2))', name: 'Honeydew II (Медовая дыня (версия 2))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>314</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Honeysuckle (Жимолость)', </v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="K99" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Honeysuckle (Жимолость)', name: 'Honeysuckle (Жимолость)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>315</v>
       </c>
       <c r="B100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Horehound (Шандра)', </v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="K100" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Horehound (Шандра)', name: 'Horehound (Шандра)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" t="s">
         <v>316</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Huckleberry (Хаклберри)', </v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="K101" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Huckleberry (Хаклберри)', name: 'Huckleberry (Хаклберри)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>317</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Irish Cream (Ирландские сливки)', </v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="K102" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Irish Cream (Ирландские сливки)', name: 'Irish Cream (Ирландские сливки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>318</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Jackfruit (Джекфрут)', </v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="K103" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Jackfruit (Джекфрут)', name: 'Jackfruit (Джекфрут)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" t="s">
         <v>319</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Jamaican Rum (Ямайский ром)', </v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="K104" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Jamaican Rum (Ямайский ром)', name: 'Jamaican Rum (Ямайский ром)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" t="s">
         <v>320</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Kalua and Cream (Калуа и сливки)', </v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="K105" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Kalua and Cream (Калуа и сливки)', name: 'Kalua and Cream (Калуа и сливки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" t="s">
         <v>321</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Kentucky Bourbon (Бурбон из Кентукки)', </v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="K106" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Kentucky Bourbon (Бурбон из Кентукки)', name: 'Kentucky Bourbon (Бурбон из Кентукки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>322</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Key Lime (Лайм)', </v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="K107" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Key Lime (Лайм)', name: 'Key Lime (Лайм)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>323</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Kiwi (Киви)', </v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="K108" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Kiwi (Киви)', name: 'Kiwi (Киви)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>324</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Kiwi (Double) (Киви (двойной))', </v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="K109" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Kiwi (Double) (Киви (двойной))', name: 'Kiwi (Double) (Киви (двойной))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>325</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Koolada 10 PG (Кулада)', </v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="K110" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Koolada 10 PG (Кулада)', name: 'Koolada 10 PG (Кулада)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>326</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lemon (water soluble) (Лимон)', </v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="K111" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lemon (water soluble) (Лимон)', name: 'Lemon (water soluble) (Лимон)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>327</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lemon 2 (Лимон (Версия 2))', </v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="K112" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lemon 2 (Лимон (Версия 2))', name: 'Lemon 2 (Лимон (Версия 2))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>328</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lemon Lime (Лимон-лайм)', </v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="K113" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lemon Lime (Лимон-лайм)', name: 'Lemon Lime (Лимон-лайм)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" t="s">
         <v>329</v>
       </c>
       <c r="B114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lemon Lime 2 (Лимон лайм (версия 2))', </v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="K114" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lemon Lime 2 (Лимон лайм (версия 2))', name: 'Lemon Lime 2 (Лимон лайм (версия 2))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" t="s">
         <v>330</v>
       </c>
       <c r="B115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lemonade Cookie (Лимонадное печенье)', </v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="K115" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lemonade Cookie (Лимонадное печенье)', name: 'Lemonade Cookie (Лимонадное печенье)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>127</v>
       </c>
       <c r="B116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lucky Leprechaun Cereal (Зефирные хлопья)', </v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="K116" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lucky Leprechaun Cereal (Зефирные хлопья)', name: 'Lucky Leprechaun Cereal (Зефирные хлопья)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" t="s">
         <v>331</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Lychee (Личи)', </v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="K117" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Lychee (Личи)', name: 'Lychee (Личи)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" t="s">
         <v>332</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'M Type Premium (Эм тайп премиум (табак))', </v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="K118" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'M Type Premium (Эм тайп премиум (табак))', name: 'M Type Premium (Эм тайп премиум (табак))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>333</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Malted milk (Сухое молоко)', </v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="K119" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Malted milk (Сухое молоко)', name: 'Malted milk (Сухое молоко)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>334</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Mango (Манго)', </v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="K120" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Mango (Манго)', name: 'Mango (Манго)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>335</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Maple Extract (Кленовый экстракт)', </v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="K121" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Maple Extract (Кленовый экстракт)', name: 'Maple Extract (Кленовый экстракт)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" t="s">
         <v>336</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Maple Syrup (Кленовый сироп)', </v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="K122" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Maple Syrup (Кленовый сироп)', name: 'Maple Syrup (Кленовый сироп)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>337</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Marshmallow (Маршмеллоу)', </v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="K123" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Marshmallow (Маршмеллоу)', name: 'Marshmallow (Маршмеллоу)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>338</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Mary Jane (Мери Джейн)', </v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="K124" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Mary Jane (Мери Джейн)', name: 'Mary Jane (Мери Джейн)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" t="s">
         <v>339</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Menthol liquid (Ментол)', </v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="K125" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Menthol liquid (Ментол)', name: 'Menthol liquid (Ментол)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>340</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Meringue (Безе)', </v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="K126" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Meringue (Безе)', name: 'Meringue (Безе)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" t="s">
         <v>341</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Milk Chocolate (Молочный шоколад)', </v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="K127" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Milk Chocolate (Молочный шоколад)', name: 'Milk Chocolate (Молочный шоколад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" t="s">
         <v>342</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Mojito Havana (Мохито)', </v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="K128" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Mojito Havana (Мохито)', name: 'Mojito Havana (Мохито)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" t="s">
         <v>343</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">'Molasses (Меласса)', </v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="K129" t="str">
+        <f t="shared" si="3"/>
+        <v>{id: 'Molasses (Меласса)', name: 'Molasses (Меласса)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" t="s">
         <v>344</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" ref="B130:B193" si="2">CONCATENATE("'",A130,"', ")</f>
+        <f t="shared" ref="B130:B193" si="4">CONCATENATE("'",A130,"', ")</f>
         <v xml:space="preserve">'Musk Candy (Конфеты Musk Lifesaver)', </v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="K130" t="str">
+        <f t="shared" ref="K130:K193" si="5">CONCATENATE($F$1,$G$1,B130,$H$1,B130,$I$1)</f>
+        <v>{id: 'Musk Candy (Конфеты Musk Lifesaver)', name: 'Musk Candy (Конфеты Musk Lifesaver)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131" t="s">
         <v>345</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Nectarine (Нектарин)', </v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="K131" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Nectarine (Нектарин)', name: 'Nectarine (Нектарин)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132" t="s">
         <v>346</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Oatmeal Cookie (Овсянное печенье)', </v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="K132" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Oatmeal Cookie (Овсянное печенье)', name: 'Oatmeal Cookie (Овсянное печенье)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133" t="s">
         <v>347</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Orange Cream (Апельсиновый крем)', </v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="K133" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Orange Cream (Апельсиновый крем)', name: 'Orange Cream (Апельсиновый крем)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" t="s">
         <v>348</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Orange Mandarin (Мандарин)', </v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="K134" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Orange Mandarin (Мандарин)', name: 'Orange Mandarin (Мандарин)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" t="s">
         <v>349</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pancake (Панкейк)', </v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="K135" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pancake (Панкейк)', name: 'Pancake (Панкейк)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" t="s">
         <v>350</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Papaya (Папайя)', </v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="K136" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Papaya (Папайя)', name: 'Papaya (Папайя)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" t="s">
         <v>351</v>
       </c>
       <c r="B137" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Passion Fruit (Маракуйя)', </v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="K137" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Passion Fruit (Маракуйя)', name: 'Passion Fruit (Маракуйя)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" t="s">
         <v>352</v>
       </c>
       <c r="B138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Peach (Персик)', </v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="K138" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Peach (Персик)', name: 'Peach (Персик)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" t="s">
         <v>353</v>
       </c>
       <c r="B139" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Peach (Juicy) (Сок персика)', </v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="K139" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Peach (Juicy) (Сок персика)', name: 'Peach (Juicy) (Сок персика)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" t="s">
         <v>354</v>
       </c>
       <c r="B140" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Peanut Butter (Арахисовое масло)', </v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="K140" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Peanut Butter (Арахисовое масло)', name: 'Peanut Butter (Арахисовое масло)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" t="s">
         <v>355</v>
       </c>
       <c r="B141" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pear (Груша)', </v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="K141" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pear (Груша)', name: 'Pear (Груша)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" t="s">
         <v>356</v>
       </c>
       <c r="B142" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pear Candy (Грушевые конфеты)', </v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="K142" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pear Candy (Грушевые конфеты)', name: 'Pear Candy (Грушевые конфеты)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143" t="s">
         <v>357</v>
       </c>
       <c r="B143" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pecan (Орех Пекан)', </v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="K143" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pecan (Орех Пекан)', name: 'Pecan (Орех Пекан)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" t="s">
         <v>358</v>
       </c>
       <c r="B144" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Peppermint (Перечная мята)', </v>
       </c>
-    </row>
-    <row r="145" spans="1:2">
+      <c r="K144" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Peppermint (Перечная мята)', name: 'Peppermint (Перечная мята)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145" t="s">
         <v>359</v>
       </c>
       <c r="B145" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pie Crust (Корочка пирога)', </v>
       </c>
-    </row>
-    <row r="146" spans="1:2">
+      <c r="K145" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pie Crust (Корочка пирога)', name: 'Pie Crust (Корочка пирога)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146" t="s">
         <v>161</v>
       </c>
       <c r="B146" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pina Colada (Пина Колада)', </v>
       </c>
-    </row>
-    <row r="147" spans="1:2">
+      <c r="K146" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pina Colada (Пина Колада)', name: 'Pina Colada (Пина Колада)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147" t="s">
         <v>360</v>
       </c>
       <c r="B147" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pineapple (Ананас)', </v>
       </c>
-    </row>
-    <row r="148" spans="1:2">
+      <c r="K147" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pineapple (Ананас)', name: 'Pineapple (Ананас)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148" t="s">
         <v>361</v>
       </c>
       <c r="B148" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pistachio (Фисташки)', </v>
       </c>
-    </row>
-    <row r="149" spans="1:2">
+      <c r="K148" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pistachio (Фисташки)', name: 'Pistachio (Фисташки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149" t="s">
         <v>362</v>
       </c>
       <c r="B149" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Plum (Слива)', </v>
       </c>
-    </row>
-    <row r="150" spans="1:2">
+      <c r="K149" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Plum (Слива)', name: 'Plum (Слива)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150" t="s">
         <v>363</v>
       </c>
       <c r="B150" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pomegranate (Гранат)', </v>
       </c>
-    </row>
-    <row r="151" spans="1:2">
+      <c r="K150" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pomegranate (Гранат)', name: 'Pomegranate (Гранат)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151" t="s">
         <v>364</v>
       </c>
       <c r="B151" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Pomegranate Deluxe (Гранат (делюкс))', </v>
       </c>
-    </row>
-    <row r="152" spans="1:2">
+      <c r="K151" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Pomegranate Deluxe (Гранат (делюкс))', name: 'Pomegranate Deluxe (Гранат (делюкс))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152" t="s">
         <v>167</v>
       </c>
       <c r="B152" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Popcorn (Попкорн)', </v>
       </c>
-    </row>
-    <row r="153" spans="1:2">
+      <c r="K152" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Popcorn (Попкорн)', name: 'Popcorn (Попкорн)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153" t="s">
         <v>365</v>
       </c>
       <c r="B153" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Quince (Айва)', </v>
       </c>
-    </row>
-    <row r="154" spans="1:2">
+      <c r="K153" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Quince (Айва)', name: 'Quince (Айва)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154" t="s">
         <v>366</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Rainbow Drops (Скиттлс)', </v>
       </c>
-    </row>
-    <row r="155" spans="1:2">
+      <c r="K154" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Rainbow Drops (Скиттлс)', name: 'Rainbow Drops (Скиттлс)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" t="s">
         <v>367</v>
       </c>
       <c r="B155" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Raisin (Изюм)', </v>
       </c>
-    </row>
-    <row r="156" spans="1:2">
+      <c r="K155" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Raisin (Изюм)', name: 'Raisin (Изюм)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156" t="s">
         <v>368</v>
       </c>
       <c r="B156" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Raspberry (Малина)', </v>
       </c>
-    </row>
-    <row r="157" spans="1:2">
+      <c r="K156" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Raspberry (Малина)', name: 'Raspberry (Малина)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157" t="s">
         <v>369</v>
       </c>
       <c r="B157" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Raspberry (Sweet) (Сладкая малина)', </v>
       </c>
-    </row>
-    <row r="158" spans="1:2">
+      <c r="K157" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Raspberry (Sweet) (Сладкая малина)', name: 'Raspberry (Sweet) (Сладкая малина)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
       <c r="A158" t="s">
         <v>370</v>
       </c>
       <c r="B158" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Red Licorice (Красная лакрица)', </v>
       </c>
-    </row>
-    <row r="159" spans="1:2">
+      <c r="K158" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Red Licorice (Красная лакрица)', name: 'Red Licorice (Красная лакрица)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159" t="s">
         <v>371</v>
       </c>
       <c r="B159" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Red Type II Blend (Ред тайп (табак))', </v>
       </c>
-    </row>
-    <row r="160" spans="1:2">
+      <c r="K159" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Red Type II Blend (Ред тайп (табак))', name: 'Red Type II Blend (Ред тайп (табак))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160" t="s">
         <v>372</v>
       </c>
       <c r="B160" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Rice Crunchies (Рисовые хлопья)', </v>
       </c>
-    </row>
-    <row r="161" spans="1:2">
+      <c r="K160" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Rice Crunchies (Рисовые хлопья)', name: 'Rice Crunchies (Рисовые хлопья)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161" t="s">
         <v>373</v>
       </c>
       <c r="B161" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Ripe Banana (Спелый банан)', </v>
       </c>
-    </row>
-    <row r="162" spans="1:2">
+      <c r="K161" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Ripe Banana (Спелый банан)', name: 'Ripe Banana (Спелый банан)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
       <c r="A162" t="s">
         <v>374</v>
       </c>
       <c r="B162" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Root beer flavor (pg) (Рутбир)', </v>
       </c>
-    </row>
-    <row r="163" spans="1:2">
+      <c r="K162" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Root beer flavor (pg) (Рутбир)', name: 'Root beer flavor (pg) (Рутбир)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
       <c r="A163" t="s">
         <v>375</v>
       </c>
       <c r="B163" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Root Beer Float (Рутбир Float)', </v>
       </c>
-    </row>
-    <row r="164" spans="1:2">
+      <c r="K163" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Root Beer Float (Рутбир Float)', name: 'Root Beer Float (Рутбир Float)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
       <c r="A164" t="s">
         <v>376</v>
       </c>
       <c r="B164" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'RY4 Double (RY4 (Табак (двойной)))', </v>
       </c>
-    </row>
-    <row r="165" spans="1:2">
+      <c r="K164" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'RY4 Double (RY4 (Табак (двойной)))', name: 'RY4 Double (RY4 (Табак (двойной)))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
       <c r="A165" t="s">
         <v>377</v>
       </c>
       <c r="B165" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'RY4 Type (RY4 (Табак))', </v>
       </c>
-    </row>
-    <row r="166" spans="1:2">
+      <c r="K165" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'RY4 Type (RY4 (Табак))', name: 'RY4 Type (RY4 (Табак))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
       <c r="A166" t="s">
         <v>378</v>
       </c>
       <c r="B166" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Slim Mint Cookie (Мятное печенье)', </v>
       </c>
-    </row>
-    <row r="167" spans="1:2">
+      <c r="K166" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Slim Mint Cookie (Мятное печенье)', name: 'Slim Mint Cookie (Мятное печенье)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
       <c r="A167" t="s">
         <v>379</v>
       </c>
       <c r="B167" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Smooth (Smooth)', </v>
       </c>
-    </row>
-    <row r="168" spans="1:2">
+      <c r="K167" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Smooth (Smooth)', name: 'Smooth (Smooth)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
       <c r="A168" t="s">
         <v>380</v>
       </c>
       <c r="B168" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Sour (Кислый)', </v>
       </c>
-    </row>
-    <row r="169" spans="1:2">
+      <c r="K168" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Sour (Кислый)', name: 'Sour (Кислый)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
       <c r="A169" t="s">
         <v>381</v>
       </c>
       <c r="B169" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Spearmint (Мята колосистая)', </v>
       </c>
-    </row>
-    <row r="170" spans="1:2">
+      <c r="K169" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Spearmint (Мята колосистая)', name: 'Spearmint (Мята колосистая)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
       <c r="A170" t="s">
         <v>382</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Strawberries and Cream (Клубника со сливками)', </v>
       </c>
-    </row>
-    <row r="171" spans="1:2">
+      <c r="K170" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Strawberries and Cream (Клубника со сливками)', name: 'Strawberries and Cream (Клубника со сливками)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
       <c r="A171" t="s">
         <v>383</v>
       </c>
       <c r="B171" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Strawberry (Клубника)', </v>
       </c>
-    </row>
-    <row r="172" spans="1:2">
+      <c r="K171" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Strawberry (Клубника)', name: 'Strawberry (Клубника)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
       <c r="A172" t="s">
         <v>384</v>
       </c>
       <c r="B172" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Strawberry (Ripe) (Спелая клубника)', </v>
       </c>
-    </row>
-    <row r="173" spans="1:2">
+      <c r="K172" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Strawberry (Ripe) (Спелая клубника)', name: 'Strawberry (Ripe) (Спелая клубника)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
       <c r="A173" t="s">
         <v>385</v>
       </c>
       <c r="B173" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Swedish Gummy (Шведский гамми)', </v>
       </c>
-    </row>
-    <row r="174" spans="1:2">
+      <c r="K173" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Swedish Gummy (Шведский гамми)', name: 'Swedish Gummy (Шведский гамми)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
       <c r="A174" t="s">
         <v>386</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Sweet and Tart (Кофеты Sweet Tart (Холодок))', </v>
       </c>
-    </row>
-    <row r="175" spans="1:2">
+      <c r="K174" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Sweet and Tart (Кофеты Sweet Tart (Холодок))', name: 'Sweet and Tart (Кофеты Sweet Tart (Холодок))', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
       <c r="A175" t="s">
         <v>387</v>
       </c>
       <c r="B175" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Sweet Cream (Сладкий крем)', </v>
       </c>
-    </row>
-    <row r="176" spans="1:2">
+      <c r="K175" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Sweet Cream (Сладкий крем)', name: 'Sweet Cream (Сладкий крем)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
       <c r="A176" t="s">
         <v>388</v>
       </c>
       <c r="B176" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Sweet Tea (Сладкий чай)', </v>
       </c>
-    </row>
-    <row r="177" spans="1:2">
+      <c r="K176" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Sweet Tea (Сладкий чай)', name: 'Sweet Tea (Сладкий чай)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11">
       <c r="A177" t="s">
         <v>389</v>
       </c>
       <c r="B177" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Sweetener (Подсластитель)', </v>
       </c>
-    </row>
-    <row r="178" spans="1:2">
+      <c r="K177" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Sweetener (Подсластитель)', name: 'Sweetener (Подсластитель)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11">
       <c r="A178" t="s">
         <v>390</v>
       </c>
       <c r="B178" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Tiramisu (Тирамису)', </v>
       </c>
-    </row>
-    <row r="179" spans="1:2">
+      <c r="K178" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Tiramisu (Тирамису)', name: 'Tiramisu (Тирамису)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11">
       <c r="A179" t="s">
         <v>391</v>
       </c>
       <c r="B179" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Toasted Almond (Жаренный миндаль)', </v>
       </c>
-    </row>
-    <row r="180" spans="1:2">
+      <c r="K179" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Toasted Almond (Жаренный миндаль)', name: 'Toasted Almond (Жаренный миндаль)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11">
       <c r="A180" t="s">
         <v>392</v>
       </c>
       <c r="B180" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Toasted Marshmallow (Поджареный зефир)', </v>
       </c>
-    </row>
-    <row r="181" spans="1:2">
+      <c r="K180" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Toasted Marshmallow (Поджареный зефир)', name: 'Toasted Marshmallow (Поджареный зефир)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11">
       <c r="A181" t="s">
         <v>393</v>
       </c>
       <c r="B181" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Tutti-Frutti (Тутти-фрутти)', </v>
       </c>
-    </row>
-    <row r="182" spans="1:2">
+      <c r="K181" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Tutti-Frutti (Тутти-фрутти)', name: 'Tutti-Frutti (Тутти-фрутти)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11">
       <c r="A182" t="s">
         <v>394</v>
       </c>
       <c r="B182" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla (Bourbon) (Ваниль бурбон)', </v>
       </c>
-    </row>
-    <row r="183" spans="1:2">
+      <c r="K182" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla (Bourbon) (Ваниль бурбон)', name: 'Vanilla (Bourbon) (Ваниль бурбон)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11">
       <c r="A183" t="s">
         <v>395</v>
       </c>
       <c r="B183" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla Bean Gelato (Ванильный заварной крем)', </v>
       </c>
-    </row>
-    <row r="184" spans="1:2">
+      <c r="K183" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla Bean Gelato (Ванильный заварной крем)', name: 'Vanilla Bean Gelato (Ванильный заварной крем)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11">
       <c r="A184" t="s">
         <v>396</v>
       </c>
       <c r="B184" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla Bean Ice Cream (Ванильное мороженное)', </v>
       </c>
-    </row>
-    <row r="185" spans="1:2">
+      <c r="K184" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla Bean Ice Cream (Ванильное мороженное)', name: 'Vanilla Bean Ice Cream (Ванильное мороженное)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11">
       <c r="A185" t="s">
         <v>397</v>
       </c>
       <c r="B185" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla Cupcake (Ванильный пирог)', </v>
       </c>
-    </row>
-    <row r="186" spans="1:2">
+      <c r="K185" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla Cupcake (Ванильный пирог)', name: 'Vanilla Cupcake (Ванильный пирог)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11">
       <c r="A186" t="s">
         <v>398</v>
       </c>
       <c r="B186" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla Custard (Ванильный кастард)', </v>
       </c>
-    </row>
-    <row r="187" spans="1:2">
+      <c r="K186" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla Custard (Ванильный кастард)', name: 'Vanilla Custard (Ванильный кастард)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11">
       <c r="A187" t="s">
         <v>399</v>
       </c>
       <c r="B187" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanilla Swirl (Ванильный рожок)', </v>
       </c>
-    </row>
-    <row r="188" spans="1:2">
+      <c r="K187" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanilla Swirl (Ванильный рожок)', name: 'Vanilla Swirl (Ванильный рожок)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11">
       <c r="A188" t="s">
         <v>400</v>
       </c>
       <c r="B188" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Vanillin 10 (PG) (Ванилин)', </v>
       </c>
-    </row>
-    <row r="189" spans="1:2">
+      <c r="K188" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Vanillin 10 (PG) (Ванилин)', name: 'Vanillin 10 (PG) (Ванилин)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11">
       <c r="A189" t="s">
         <v>401</v>
       </c>
       <c r="B189" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Waffle (Вафли)', </v>
       </c>
-    </row>
-    <row r="190" spans="1:2">
+      <c r="K189" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Waffle (Вафли)', name: 'Waffle (Вафли)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11">
       <c r="A190" t="s">
         <v>211</v>
       </c>
       <c r="B190" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Waffle (Belgian) (Бельгийские вафли)', </v>
       </c>
-    </row>
-    <row r="191" spans="1:2">
+      <c r="K190" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Waffle (Belgian) (Бельгийские вафли)', name: 'Waffle (Belgian) (Бельгийские вафли)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11">
       <c r="A191" t="s">
         <v>402</v>
       </c>
       <c r="B191" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Watermelon (Арбуз)', </v>
       </c>
-    </row>
-    <row r="192" spans="1:2">
+      <c r="K191" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Watermelon (Арбуз)', name: 'Watermelon (Арбуз)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11">
       <c r="A192" t="s">
         <v>403</v>
       </c>
       <c r="B192" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Watermelon Candy (Арбузные леденцы)', </v>
       </c>
-    </row>
-    <row r="193" spans="1:2">
+      <c r="K192" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Watermelon Candy (Арбузные леденцы)', name: 'Watermelon Candy (Арбузные леденцы)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
       <c r="A193" t="s">
         <v>404</v>
       </c>
       <c r="B193" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">'Western (Вестерн)', </v>
       </c>
-    </row>
-    <row r="194" spans="1:2">
+      <c r="K193" t="str">
+        <f t="shared" si="5"/>
+        <v>{id: 'Western (Вестерн)', name: 'Western (Вестерн)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
       <c r="A194" t="s">
         <v>405</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" ref="B194:B197" si="3">CONCATENATE("'",A194,"', ")</f>
+        <f t="shared" ref="B194:B197" si="6">CONCATENATE("'",A194,"', ")</f>
         <v xml:space="preserve">'Whipped Cream (Взбитые сливки)', </v>
       </c>
-    </row>
-    <row r="195" spans="1:2">
+      <c r="K194" t="str">
+        <f t="shared" ref="K194:K197" si="7">CONCATENATE($F$1,$G$1,B194,$H$1,B194,$I$1)</f>
+        <v>{id: 'Whipped Cream (Взбитые сливки)', name: 'Whipped Cream (Взбитые сливки)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
       <c r="A195" t="s">
         <v>406</v>
       </c>
       <c r="B195" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">'White Chocolate (Белый шоколад)', </v>
       </c>
-    </row>
-    <row r="196" spans="1:2">
+      <c r="K195" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'White Chocolate (Белый шоколад)', name: 'White Chocolate (Белый шоколад)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
       <c r="A196" t="s">
         <v>407</v>
       </c>
       <c r="B196" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">'Wintergreen (Мятные кофеты)', </v>
       </c>
-    </row>
-    <row r="197" spans="1:2">
+      <c r="K196" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Wintergreen (Мятные кофеты)', name: 'Wintergreen (Мятные кофеты)', isSelected: false },</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
       <c r="A197" t="s">
         <v>219</v>
       </c>
       <c r="B197" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">'Yam (Ямс)', </v>
+      </c>
+      <c r="K197" t="str">
+        <f t="shared" si="7"/>
+        <v>{id: 'Yam (Ямс)', name: 'Yam (Ямс)', isSelected: false },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EVERYTHING IS WORK!!! FINALLY MPHACA
</commit_message>
<xml_diff>
--- a/список ароматизаторов.xlsx
+++ b/список ароматизаторов.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="413">
   <si>
     <t>A</t>
   </si>
@@ -6143,7 +6143,10 @@
     <t xml:space="preserve">name: </t>
   </si>
   <si>
-    <t>isSelected: false },</t>
+    <t>isSelected: false</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> },</t>
   </si>
 </sst>
 </file>
@@ -8297,24 +8300,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K197"/>
+  <dimension ref="A1:L197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="M168" sqref="M168"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>220</v>
       </c>
       <c r="B1" t="str">
-        <f>CONCATENATE("'",A1,"', ")</f>
-        <v xml:space="preserve">'Absinthe (Абсент)', </v>
+        <f>CONCATENATE("'",A1,"'")</f>
+        <v>'Absinthe (Абсент)'</v>
       </c>
       <c r="F1" t="s">
         <v>409</v>
@@ -8328,2557 +8332,3348 @@
       <c r="I1" t="s">
         <v>411</v>
       </c>
+      <c r="J1" t="s">
+        <v>412</v>
+      </c>
       <c r="K1" t="str">
-        <f>CONCATENATE($F$1,$G$1,B1,$H$1,B1,$I$1)</f>
-        <v>{id: 'Absinthe (Абсент)', name: 'Absinthe (Абсент)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <f>CONCATENATE($F$1,$H$1,B1,$J$1)</f>
+        <v>{name: 'Absinthe (Абсент)' },</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE($F$1,$G$1,C1,$H$1,C1,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>221</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B65" si="0">CONCATENATE("'",A2,"', ")</f>
-        <v xml:space="preserve">'Acai (Ягода асаи)', </v>
+        <f t="shared" ref="B2:B65" si="0">CONCATENATE("'",A2,"'")</f>
+        <v>'Acai (Ягода асаи)'</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K65" si="1">CONCATENATE($F$1,$G$1,B2,$H$1,B2,$I$1)</f>
-        <v>{id: 'Acai (Ягода асаи)', name: 'Acai (Ягода асаи)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <f t="shared" ref="K2:K65" si="1">CONCATENATE($F$1,$H$1,B2,$J$1)</f>
+        <v>{name: 'Acai (Ягода асаи)' },</v>
+      </c>
+      <c r="L2" t="str">
+        <f>CONCATENATE($F$1,$G$1,C2,$H$1,C2,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>222</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Acetyl Pyrazine (Ацетил пиразин)', </v>
+        <v>'Acetyl Pyrazine (Ацетил пиразин)'</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Acetyl Pyrazine (Ацетил пиразин)', name: 'Acetyl Pyrazine (Ацетил пиразин)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>{name: 'Acetyl Pyrazine (Ацетил пиразин)' },</v>
+      </c>
+      <c r="L3" t="str">
+        <f>CONCATENATE($F$1,$G$1,C3,$H$1,C3,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>223</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Almond (Миндаль)', </v>
+        <v>'Almond (Миндаль)'</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Almond (Миндаль)', name: 'Almond (Миндаль)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>{name: 'Almond (Миндаль)' },</v>
+      </c>
+      <c r="L4" t="str">
+        <f>CONCATENATE($F$1,$G$1,C4,$H$1,C4,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>224</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Apple (Яблоко)', </v>
+        <v>'Apple (Яблоко)'</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Apple (Яблоко)', name: 'Apple (Яблоко)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>{name: 'Apple (Яблоко)' },</v>
+      </c>
+      <c r="L5" t="str">
+        <f>CONCATENATE($F$1,$G$1,C5,$H$1,C5,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>225</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Apple (tart granny smith) (Яблоко (Гренни Смит))', </v>
+        <v>'Apple (tart granny smith) (Яблоко (Гренни Смит))'</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Apple (tart granny smith) (Яблоко (Гренни Смит))', name: 'Apple (tart granny smith) (Яблоко (Гренни Смит))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>{name: 'Apple (tart granny smith) (Яблоко (Гренни Смит))' },</v>
+      </c>
+      <c r="L6" t="str">
+        <f>CONCATENATE($F$1,$G$1,C6,$H$1,C6,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>226</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Apple Candy (Яблочный мармелад)', </v>
+        <v>'Apple Candy (Яблочный мармелад)'</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Apple Candy (Яблочный мармелад)', name: 'Apple Candy (Яблочный мармелад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>{name: 'Apple Candy (Яблочный мармелад)' },</v>
+      </c>
+      <c r="L7" t="str">
+        <f>CONCATENATE($F$1,$G$1,C7,$H$1,C7,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>227</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Apple Pie (Яблочный пирог)', </v>
+        <v>'Apple Pie (Яблочный пирог)'</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Apple Pie (Яблочный пирог)', name: 'Apple Pie (Яблочный пирог)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>{name: 'Apple Pie (Яблочный пирог)' },</v>
+      </c>
+      <c r="L8" t="str">
+        <f>CONCATENATE($F$1,$G$1,C8,$H$1,C8,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>228</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Apricot (Абрикос)', </v>
+        <v>'Apricot (Абрикос)'</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Apricot (Абрикос)', name: 'Apricot (Абрикос)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>{name: 'Apricot (Абрикос)' },</v>
+      </c>
+      <c r="L9" t="str">
+        <f>CONCATENATE($F$1,$G$1,C9,$H$1,C9,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>229</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Banana (Банан)', </v>
+        <v>'Banana (Банан)'</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Banana (Банан)', name: 'Banana (Банан)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>{name: 'Banana (Банан)' },</v>
+      </c>
+      <c r="L10" t="str">
+        <f>CONCATENATE($F$1,$G$1,C10,$H$1,C10,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>230</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Banana Cream (Банановый крем)', </v>
+        <v>'Banana Cream (Банановый крем)'</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Banana Cream (Банановый крем)', name: 'Banana Cream (Банановый крем)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>{name: 'Banana Cream (Банановый крем)' },</v>
+      </c>
+      <c r="L11" t="str">
+        <f>CONCATENATE($F$1,$G$1,C11,$H$1,C11,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>231</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Banana Nut Bread (Банановый хлеб)', </v>
+        <v>'Banana Nut Bread (Банановый хлеб)'</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Banana Nut Bread (Банановый хлеб)', name: 'Banana Nut Bread (Банановый хлеб)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>{name: 'Banana Nut Bread (Банановый хлеб)' },</v>
+      </c>
+      <c r="L12" t="str">
+        <f>CONCATENATE($F$1,$G$1,C12,$H$1,C12,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>232</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bananas Foster (Банановый фостер)', </v>
+        <v>'Bananas Foster (Банановый фостер)'</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bananas Foster (Банановый фостер)', name: 'Bananas Foster (Банановый фостер)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>{name: 'Bananas Foster (Банановый фостер)' },</v>
+      </c>
+      <c r="L13" t="str">
+        <f>CONCATENATE($F$1,$G$1,C13,$H$1,C13,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>233</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bavarian Cream (Баварский крем)', </v>
+        <v>'Bavarian Cream (Баварский крем)'</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bavarian Cream (Баварский крем)', name: 'Bavarian Cream (Баварский крем)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>{name: 'Bavarian Cream (Баварский крем)' },</v>
+      </c>
+      <c r="L14" t="str">
+        <f>CONCATENATE($F$1,$G$1,C14,$H$1,C14,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>234</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Berry Crunch (Ягодные хлопья)', </v>
+        <v>'Berry Crunch (Ягодные хлопья)'</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Berry Crunch (Ягодные хлопья)', name: 'Berry Crunch (Ягодные хлопья)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>{name: 'Berry Crunch (Ягодные хлопья)' },</v>
+      </c>
+      <c r="L15" t="str">
+        <f>CONCATENATE($F$1,$G$1,C15,$H$1,C15,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>235</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bitter Nut Extra (Горький орех)', </v>
+        <v>'Bitter Nut Extra (Горький орех)'</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bitter Nut Extra (Горький орех)', name: 'Bitter Nut Extra (Горький орех)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>{name: 'Bitter Nut Extra (Горький орех)' },</v>
+      </c>
+      <c r="L16" t="str">
+        <f>CONCATENATE($F$1,$G$1,C16,$H$1,C16,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>236</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bittersweet Chocolate (Биттерсвит шоколад)', </v>
+        <v>'Bittersweet Chocolate (Биттерсвит шоколад)'</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bittersweet Chocolate (Биттерсвит шоколад)', name: 'Bittersweet Chocolate (Биттерсвит шоколад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>{name: 'Bittersweet Chocolate (Биттерсвит шоколад)' },</v>
+      </c>
+      <c r="L17" t="str">
+        <f>CONCATENATE($F$1,$G$1,C17,$H$1,C17,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>237</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Black Cherry (Черешня)', </v>
+        <v>'Black Cherry (Черешня)'</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Black Cherry (Черешня)', name: 'Black Cherry (Черешня)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>{name: 'Black Cherry (Черешня)' },</v>
+      </c>
+      <c r="L18" t="str">
+        <f>CONCATENATE($F$1,$G$1,C18,$H$1,C18,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>238</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Black Currant (Черная смородина)', </v>
+        <v>'Black Currant (Черная смородина)'</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Black Currant (Черная смородина)', name: 'Black Currant (Черная смородина)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>{name: 'Black Currant (Черная смородина)' },</v>
+      </c>
+      <c r="L19" t="str">
+        <f>CONCATENATE($F$1,$G$1,C19,$H$1,C19,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>239</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Black Honey (Черный мед и табак)', </v>
+        <v>'Black Honey (Черный мед и табак)'</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Black Honey (Черный мед и табак)', name: 'Black Honey (Черный мед и табак)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>{name: 'Black Honey (Черный мед и табак)' },</v>
+      </c>
+      <c r="L20" t="str">
+        <f>CONCATENATE($F$1,$G$1,C20,$H$1,C20,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Black Tea (Черный чай)', </v>
+        <v>'Black Tea (Черный чай)'</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Black Tea (Черный чай)', name: 'Black Tea (Черный чай)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>{name: 'Black Tea (Черный чай)' },</v>
+      </c>
+      <c r="L21" t="str">
+        <f>CONCATENATE($F$1,$G$1,C21,$H$1,C21,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>240</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Blackberry (Ежевика)', </v>
+        <v>'Blackberry (Ежевика)'</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Blackberry (Ежевика)', name: 'Blackberry (Ежевика)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>{name: 'Blackberry (Ежевика)' },</v>
+      </c>
+      <c r="L22" t="str">
+        <f>CONCATENATE($F$1,$G$1,C22,$H$1,C22,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>241</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Blue Raspberry (Голубая малина)', </v>
+        <v>'Blue Raspberry (Голубая малина)'</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Blue Raspberry (Голубая малина)', name: 'Blue Raspberry (Голубая малина)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>{name: 'Blue Raspberry (Голубая малина)' },</v>
+      </c>
+      <c r="L23" t="str">
+        <f>CONCATENATE($F$1,$G$1,C23,$H$1,C23,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>242</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Blueberry (Extra) (Черника)', </v>
+        <v>'Blueberry (Extra) (Черника)'</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Blueberry (Extra) (Черника)', name: 'Blueberry (Extra) (Черника)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>{name: 'Blueberry (Extra) (Черника)' },</v>
+      </c>
+      <c r="L24" t="str">
+        <f>CONCATENATE($F$1,$G$1,C24,$H$1,C24,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>243</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Blueberry Candy (Черничные леденцы)', </v>
+        <v>'Blueberry Candy (Черничные леденцы)'</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Blueberry Candy (Черничные леденцы)', name: 'Blueberry Candy (Черничные леденцы)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>{name: 'Blueberry Candy (Черничные леденцы)' },</v>
+      </c>
+      <c r="L25" t="str">
+        <f>CONCATENATE($F$1,$G$1,C25,$H$1,C25,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>244</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Blueberry Wild (Дикая черника)', </v>
+        <v>'Blueberry Wild (Дикая черника)'</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Blueberry Wild (Дикая черника)', name: 'Blueberry Wild (Дикая черника)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>{name: 'Blueberry Wild (Дикая черника)' },</v>
+      </c>
+      <c r="L26" t="str">
+        <f>CONCATENATE($F$1,$G$1,C26,$H$1,C26,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>245</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Boysenberry (Шелковица )', </v>
+        <v>'Boysenberry (Шелковица )'</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Boysenberry (Шелковица )', name: 'Boysenberry (Шелковица )', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>{name: 'Boysenberry (Шелковица )' },</v>
+      </c>
+      <c r="L27" t="str">
+        <f>CONCATENATE($F$1,$G$1,C27,$H$1,C27,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Brandy (Бренди)', </v>
+        <v>'Brandy (Бренди)'</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Brandy (Бренди)', name: 'Brandy (Бренди)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>{name: 'Brandy (Бренди)' },</v>
+      </c>
+      <c r="L28" t="str">
+        <f>CONCATENATE($F$1,$G$1,C28,$H$1,C28,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>246</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Brown Sugar (Коричневый сахар)', </v>
+        <v>'Brown Sugar (Коричневый сахар)'</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Brown Sugar (Коричневый сахар)', name: 'Brown Sugar (Коричневый сахар)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>{name: 'Brown Sugar (Коричневый сахар)' },</v>
+      </c>
+      <c r="L29" t="str">
+        <f>CONCATENATE($F$1,$G$1,C29,$H$1,C29,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>247</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bubblegum (Жвачка)', </v>
+        <v>'Bubblegum (Жвачка)'</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bubblegum (Жвачка)', name: 'Bubblegum (Жвачка)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>{name: 'Bubblegum (Жвачка)' },</v>
+      </c>
+      <c r="L30" t="str">
+        <f>CONCATENATE($F$1,$G$1,C30,$H$1,C30,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>248</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Bubblegum (Fruity) (Жвачка (Фруктовая))', </v>
+        <v>'Bubblegum (Fruity) (Жвачка (Фруктовая))'</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Bubblegum (Fruity) (Жвачка (Фруктовая))', name: 'Bubblegum (Fruity) (Жвачка (Фруктовая))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>{name: 'Bubblegum (Fruity) (Жвачка (Фруктовая))' },</v>
+      </c>
+      <c r="L31" t="str">
+        <f>CONCATENATE($F$1,$G$1,C31,$H$1,C31,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>249</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Butter (Масло)', </v>
+        <v>'Butter (Масло)'</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Butter (Масло)', name: 'Butter (Масло)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>{name: 'Butter (Масло)' },</v>
+      </c>
+      <c r="L32" t="str">
+        <f>CONCATENATE($F$1,$G$1,C32,$H$1,C32,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>250</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Butterscotch (Ирис)', </v>
+        <v>'Butterscotch (Ирис)'</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Butterscotch (Ирис)', name: 'Butterscotch (Ирис)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>{name: 'Butterscotch (Ирис)' },</v>
+      </c>
+      <c r="L33" t="str">
+        <f>CONCATENATE($F$1,$G$1,C33,$H$1,C33,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>251</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cantaloupe (Канталупа)', </v>
+        <v>'Cantaloupe (Канталупа)'</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cantaloupe (Канталупа)', name: 'Cantaloupe (Канталупа)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>{name: 'Cantaloupe (Канталупа)' },</v>
+      </c>
+      <c r="L34" t="str">
+        <f>CONCATENATE($F$1,$G$1,C34,$H$1,C34,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>252</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cappucсino (Каппучино)', </v>
+        <v>'Cappucсino (Каппучино)'</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cappucсino (Каппучино)', name: 'Cappucсino (Каппучино)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>{name: 'Cappucсino (Каппучино)' },</v>
+      </c>
+      <c r="L35" t="str">
+        <f>CONCATENATE($F$1,$G$1,C35,$H$1,C35,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>253</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Caramel (Карамель)', </v>
+        <v>'Caramel (Карамель)'</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Caramel (Карамель)', name: 'Caramel (Карамель)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>{name: 'Caramel (Карамель)' },</v>
+      </c>
+      <c r="L36" t="str">
+        <f>CONCATENATE($F$1,$G$1,C36,$H$1,C36,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>254</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Caramel (Original) (Карамель (Оригинальная))', </v>
+        <v>'Caramel (Original) (Карамель (Оригинальная))'</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Caramel (Original) (Карамель (Оригинальная))', name: 'Caramel (Original) (Карамель (Оригинальная))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>{name: 'Caramel (Original) (Карамель (Оригинальная))' },</v>
+      </c>
+      <c r="L37" t="str">
+        <f>CONCATENATE($F$1,$G$1,C37,$H$1,C37,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>255</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Caramel Candy (Карамельная конфета)', </v>
+        <v>'Caramel Candy (Карамельная конфета)'</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Caramel Candy (Карамельная конфета)', name: 'Caramel Candy (Карамельная конфета)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>{name: 'Caramel Candy (Карамельная конфета)' },</v>
+      </c>
+      <c r="L38" t="str">
+        <f>CONCATENATE($F$1,$G$1,C38,$H$1,C38,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>256</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Caramel Cappuccino (Карамель-каппучино)', </v>
+        <v>'Caramel Cappuccino (Карамель-каппучино)'</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Caramel Cappuccino (Карамель-каппучино)', name: 'Caramel Cappuccino (Карамель-каппучино)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>{name: 'Caramel Cappuccino (Карамель-каппучино)' },</v>
+      </c>
+      <c r="L39" t="str">
+        <f>CONCATENATE($F$1,$G$1,C39,$H$1,C39,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>257</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Chai Tea (Чай)', </v>
+        <v>'Chai Tea (Чай)'</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Chai Tea (Чай)', name: 'Chai Tea (Чай)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>{name: 'Chai Tea (Чай)' },</v>
+      </c>
+      <c r="L40" t="str">
+        <f>CONCATENATE($F$1,$G$1,C40,$H$1,C40,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>258</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Champagne (Шампанское)', </v>
+        <v>'Champagne (Шампанское)'</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Champagne (Шампанское)', name: 'Champagne (Шампанское)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>{name: 'Champagne (Шампанское)' },</v>
+      </c>
+      <c r="L41" t="str">
+        <f>CONCATENATE($F$1,$G$1,C41,$H$1,C41,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>259</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cheesecake (Чизкейк)', </v>
+        <v>'Cheesecake (Чизкейк)'</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cheesecake (Чизкейк)', name: 'Cheesecake (Чизкейк)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <v>{name: 'Cheesecake (Чизкейк)' },</v>
+      </c>
+      <c r="L42" t="str">
+        <f>CONCATENATE($F$1,$G$1,C42,$H$1,C42,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>260</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cheesecake (Graham Crust) (Чизкейк (корочка))', </v>
+        <v>'Cheesecake (Graham Crust) (Чизкейк (корочка))'</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cheesecake (Graham Crust) (Чизкейк (корочка))', name: 'Cheesecake (Graham Crust) (Чизкейк (корочка))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>{name: 'Cheesecake (Graham Crust) (Чизкейк (корочка))' },</v>
+      </c>
+      <c r="L43" t="str">
+        <f>CONCATENATE($F$1,$G$1,C43,$H$1,C43,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>261</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cherry Blossom (Цветущая вишня)', </v>
+        <v>'Cherry Blossom (Цветущая вишня)'</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cherry Blossom (Цветущая вишня)', name: 'Cherry Blossom (Цветущая вишня)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>{name: 'Cherry Blossom (Цветущая вишня)' },</v>
+      </c>
+      <c r="L44" t="str">
+        <f>CONCATENATE($F$1,$G$1,C44,$H$1,C44,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>262</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cherry Extract (Экстракт вишни)', </v>
+        <v>'Cherry Extract (Экстракт вишни)'</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cherry Extract (Экстракт вишни)', name: 'Cherry Extract (Экстракт вишни)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>{name: 'Cherry Extract (Экстракт вишни)' },</v>
+      </c>
+      <c r="L45" t="str">
+        <f>CONCATENATE($F$1,$G$1,C45,$H$1,C45,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Chocolate (Шоколад)', </v>
+        <v>'Chocolate (Шоколад)'</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Chocolate (Шоколад)', name: 'Chocolate (Шоколад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+        <v>{name: 'Chocolate (Шоколад)' },</v>
+      </c>
+      <c r="L46" t="str">
+        <f>CONCATENATE($F$1,$G$1,C46,$H$1,C46,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>263</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cinnamon (Корица)', </v>
+        <v>'Cinnamon (Корица)'</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cinnamon (Корица)', name: 'Cinnamon (Корица)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>{name: 'Cinnamon (Корица)' },</v>
+      </c>
+      <c r="L47" t="str">
+        <f>CONCATENATE($F$1,$G$1,C47,$H$1,C47,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>264</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cinnamon Danish (Корица датская)', </v>
+        <v>'Cinnamon Danish (Корица датская)'</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cinnamon Danish (Корица датская)', name: 'Cinnamon Danish (Корица датская)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>{name: 'Cinnamon Danish (Корица датская)' },</v>
+      </c>
+      <c r="L48" t="str">
+        <f>CONCATENATE($F$1,$G$1,C48,$H$1,C48,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>265</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cinnamon Red Hot (Корица)', </v>
+        <v>'Cinnamon Red Hot (Корица)'</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cinnamon Red Hot (Корица)', name: 'Cinnamon Red Hot (Корица)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>{name: 'Cinnamon Red Hot (Корица)' },</v>
+      </c>
+      <c r="L49" t="str">
+        <f>CONCATENATE($F$1,$G$1,C49,$H$1,C49,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>266</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cinnamon Spice (Острая корица)', </v>
+        <v>'Cinnamon Spice (Острая корица)'</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cinnamon Spice (Острая корица)', name: 'Cinnamon Spice (Острая корица)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+        <v>{name: 'Cinnamon Spice (Острая корица)' },</v>
+      </c>
+      <c r="L50" t="str">
+        <f>CONCATENATE($F$1,$G$1,C50,$H$1,C50,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>267</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cinnamon Sugar Cookie (Печенье с корицей)', </v>
+        <v>'Cinnamon Sugar Cookie (Печенье с корицей)'</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cinnamon Sugar Cookie (Печенье с корицей)', name: 'Cinnamon Sugar Cookie (Печенье с корицей)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+        <v>{name: 'Cinnamon Sugar Cookie (Печенье с корицей)' },</v>
+      </c>
+      <c r="L51" t="str">
+        <f>CONCATENATE($F$1,$G$1,C51,$H$1,C51,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>268</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Citrus Punch (Цитрусовый пунш)', </v>
+        <v>'Citrus Punch (Цитрусовый пунш)'</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Citrus Punch (Цитрусовый пунш)', name: 'Citrus Punch (Цитрусовый пунш)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+        <v>{name: 'Citrus Punch (Цитрусовый пунш)' },</v>
+      </c>
+      <c r="L52" t="str">
+        <f>CONCATENATE($F$1,$G$1,C52,$H$1,C52,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>269</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Clove (Гвоздика)', </v>
+        <v>'Clove (Гвоздика)'</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Clove (Гвоздика)', name: 'Clove (Гвоздика)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>{name: 'Clove (Гвоздика)' },</v>
+      </c>
+      <c r="L53" t="str">
+        <f>CONCATENATE($F$1,$G$1,C53,$H$1,C53,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>270</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cocoa Rounds (Шоколадные шарики)', </v>
+        <v>'Cocoa Rounds (Шоколадные шарики)'</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cocoa Rounds (Шоколадные шарики)', name: 'Cocoa Rounds (Шоколадные шарики)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>{name: 'Cocoa Rounds (Шоколадные шарики)' },</v>
+      </c>
+      <c r="L54" t="str">
+        <f>CONCATENATE($F$1,$G$1,C54,$H$1,C54,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>271</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Coconut (Кокос)', </v>
+        <v>'Coconut (Кокос)'</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Coconut (Кокос)', name: 'Coconut (Кокос)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>{name: 'Coconut (Кокос)' },</v>
+      </c>
+      <c r="L55" t="str">
+        <f>CONCATENATE($F$1,$G$1,C55,$H$1,C55,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>272</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Coconut (Extra) (Кокос (Экстра))', </v>
+        <v>'Coconut (Extra) (Кокос (Экстра))'</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Coconut (Extra) (Кокос (Экстра))', name: 'Coconut (Extra) (Кокос (Экстра))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+        <v>{name: 'Coconut (Extra) (Кокос (Экстра))' },</v>
+      </c>
+      <c r="L56" t="str">
+        <f>CONCATENATE($F$1,$G$1,C56,$H$1,C56,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>273</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Coconut Candy (Кокосовые конфеты)', </v>
+        <v>'Coconut Candy (Кокосовые конфеты)'</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Coconut Candy (Кокосовые конфеты)', name: 'Coconut Candy (Кокосовые конфеты)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+        <v>{name: 'Coconut Candy (Кокосовые конфеты)' },</v>
+      </c>
+      <c r="L57" t="str">
+        <f>CONCATENATE($F$1,$G$1,C57,$H$1,C57,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>274</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Coffee (Кофе)', </v>
+        <v>'Coffee (Кофе)'</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Coffee (Кофе)', name: 'Coffee (Кофе)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+        <v>{name: 'Coffee (Кофе)' },</v>
+      </c>
+      <c r="L58" t="str">
+        <f>CONCATENATE($F$1,$G$1,C58,$H$1,C58,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>275</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cotton Candy (Сладкая вата)', </v>
+        <v>'Cotton Candy (Сладкая вата)'</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cotton Candy (Сладкая вата)', name: 'Cotton Candy (Сладкая вата)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+        <v>{name: 'Cotton Candy (Сладкая вата)' },</v>
+      </c>
+      <c r="L59" t="str">
+        <f>CONCATENATE($F$1,$G$1,C59,$H$1,C59,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>276</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cranberry (Клюква)', </v>
+        <v>'Cranberry (Клюква)'</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cranberry (Клюква)', name: 'Cranberry (Клюква)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+        <v>{name: 'Cranberry (Клюква)' },</v>
+      </c>
+      <c r="L60" t="str">
+        <f>CONCATENATE($F$1,$G$1,C60,$H$1,C60,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>277</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cream Soda (Крем-сода)', </v>
+        <v>'Cream Soda (Крем-сода)'</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cream Soda (Крем-сода)', name: 'Cream Soda (Крем-сода)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+        <v>{name: 'Cream Soda (Крем-сода)' },</v>
+      </c>
+      <c r="L61" t="str">
+        <f>CONCATENATE($F$1,$G$1,C61,$H$1,C61,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>278</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Creme de Menthe (Сладкий мятный ликер)', </v>
+        <v>'Creme de Menthe (Сладкий мятный ликер)'</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Creme de Menthe (Сладкий мятный ликер)', name: 'Creme de Menthe (Сладкий мятный ликер)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+        <v>{name: 'Creme de Menthe (Сладкий мятный ликер)' },</v>
+      </c>
+      <c r="L62" t="str">
+        <f>CONCATENATE($F$1,$G$1,C62,$H$1,C62,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>279</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Cucumber (Огурец)', </v>
+        <v>'Cucumber (Огурец)'</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Cucumber (Огурец)', name: 'Cucumber (Огурец)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+        <v>{name: 'Cucumber (Огурец)' },</v>
+      </c>
+      <c r="L63" t="str">
+        <f>CONCATENATE($F$1,$G$1,C63,$H$1,C63,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>280</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'Dairy/Milk (Молоко)', </v>
+        <v>'Dairy/Milk (Молоко)'</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'Dairy/Milk (Молоко)', name: 'Dairy/Milk (Молоко)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>{name: 'Dairy/Milk (Молоко)' },</v>
+      </c>
+      <c r="L64" t="str">
+        <f>CONCATENATE($F$1,$G$1,C64,$H$1,C64,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>281</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">'DK Tobacco Base (Табак)', </v>
+        <v>'DK Tobacco Base (Табак)'</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="1"/>
-        <v>{id: 'DK Tobacco Base (Табак)', name: 'DK Tobacco Base (Табак)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+        <v>{name: 'DK Tobacco Base (Табак)' },</v>
+      </c>
+      <c r="L65" t="str">
+        <f>CONCATENATE($F$1,$G$1,C65,$H$1,C65,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>282</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B129" si="2">CONCATENATE("'",A66,"', ")</f>
-        <v xml:space="preserve">'Double Chocolate (Clear) (Двойной шоколад)', </v>
+        <f t="shared" ref="B66:B129" si="2">CONCATENATE("'",A66,"'")</f>
+        <v>'Double Chocolate (Clear) (Двойной шоколад)'</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" ref="K66:K129" si="3">CONCATENATE($F$1,$G$1,B66,$H$1,B66,$I$1)</f>
-        <v>{id: 'Double Chocolate (Clear) (Двойной шоколад)', name: 'Double Chocolate (Clear) (Двойной шоколад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+        <f t="shared" ref="K66:K129" si="3">CONCATENATE($F$1,$H$1,B66,$J$1)</f>
+        <v>{name: 'Double Chocolate (Clear) (Двойной шоколад)' },</v>
+      </c>
+      <c r="L66" t="str">
+        <f>CONCATENATE($F$1,$G$1,C66,$H$1,C66,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>283</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Double Chocolate (Dark) (Двойной шоколад (Темный))', </v>
+        <v>'Double Chocolate (Dark) (Двойной шоколад (Темный))'</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Double Chocolate (Dark) (Двойной шоколад (Темный))', name: 'Double Chocolate (Dark) (Двойной шоколад (Темный))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+        <v>{name: 'Double Chocolate (Dark) (Двойной шоколад (Темный))' },</v>
+      </c>
+      <c r="L67" t="str">
+        <f>CONCATENATE($F$1,$G$1,C67,$H$1,C67,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>284</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Dragonfruit (Драгонфрут (питайя))', </v>
+        <v>'Dragonfruit (Драгонфрут (питайя))'</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Dragonfruit (Драгонфрут (питайя))', name: 'Dragonfruit (Драгонфрут (питайя))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+        <v>{name: 'Dragonfruit (Драгонфрут (питайя))' },</v>
+      </c>
+      <c r="L68" t="str">
+        <f>CONCATENATE($F$1,$G$1,C68,$H$1,C68,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>285</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Dulce de Leche (Сгущенное молоко)', </v>
+        <v>'Dulce de Leche (Сгущенное молоко)'</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Dulce de Leche (Сгущенное молоко)', name: 'Dulce de Leche (Сгущенное молоко)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+        <v>{name: 'Dulce de Leche (Сгущенное молоко)' },</v>
+      </c>
+      <c r="L69" t="str">
+        <f>CONCATENATE($F$1,$G$1,C69,$H$1,C69,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>286</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Earl Grey Tea (Эрл-грей)', </v>
+        <v>'Earl Grey Tea (Эрл-грей)'</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Earl Grey Tea (Эрл-грей)', name: 'Earl Grey Tea (Эрл-грей)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+        <v>{name: 'Earl Grey Tea (Эрл-грей)' },</v>
+      </c>
+      <c r="L70" t="str">
+        <f>CONCATENATE($F$1,$G$1,C70,$H$1,C70,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>287</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Elderberry (Бузина)', </v>
+        <v>'Elderberry (Бузина)'</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Elderberry (Бузина)', name: 'Elderberry (Бузина)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+        <v>{name: 'Elderberry (Бузина)' },</v>
+      </c>
+      <c r="L71" t="str">
+        <f>CONCATENATE($F$1,$G$1,C71,$H$1,C71,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>288</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Energy Drink (Энергетический напиток)', </v>
+        <v>'Energy Drink (Энергетический напиток)'</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Energy Drink (Энергетический напиток)', name: 'Energy Drink (Энергетический напиток)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
+        <v>{name: 'Energy Drink (Энергетический напиток)' },</v>
+      </c>
+      <c r="L72" t="str">
+        <f>CONCATENATE($F$1,$G$1,C72,$H$1,C72,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>289</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'English Toffee (Тоффи)', </v>
+        <v>'English Toffee (Тоффи)'</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'English Toffee (Тоффи)', name: 'English Toffee (Тоффи)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
+        <v>{name: 'English Toffee (Тоффи)' },</v>
+      </c>
+      <c r="L73" t="str">
+        <f>CONCATENATE($F$1,$G$1,C73,$H$1,C73,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>290</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Espresso (Эспрессо)', </v>
+        <v>'Espresso (Эспрессо)'</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Espresso (Эспрессо)', name: 'Espresso (Эспрессо)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
+        <v>{name: 'Espresso (Эспрессо)' },</v>
+      </c>
+      <c r="L74" t="str">
+        <f>CONCATENATE($F$1,$G$1,C74,$H$1,C74,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>291</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Ethyl Maltol (Этил мальтол)', </v>
+        <v>'Ethyl Maltol (Этил мальтол)'</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Ethyl Maltol (Этил мальтол)', name: 'Ethyl Maltol (Этил мальтол)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
+        <v>{name: 'Ethyl Maltol (Этил мальтол)' },</v>
+      </c>
+      <c r="L75" t="str">
+        <f>CONCATENATE($F$1,$G$1,C75,$H$1,C75,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>292</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'French Vanilla (Французкая ваниль)', </v>
+        <v>'French Vanilla (Французкая ваниль)'</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'French Vanilla (Французкая ваниль)', name: 'French Vanilla (Французкая ваниль)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
+        <v>{name: 'French Vanilla (Французкая ваниль)' },</v>
+      </c>
+      <c r="L76" t="str">
+        <f>CONCATENATE($F$1,$G$1,C76,$H$1,C76,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>82</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'French Vanilla Deluxe (Французкая ваниль (Делюкс))', </v>
+        <v>'French Vanilla Deluxe (Французкая ваниль (Делюкс))'</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'French Vanilla Deluxe (Французкая ваниль (Делюкс))', name: 'French Vanilla Deluxe (Французкая ваниль (Делюкс))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
+        <v>{name: 'French Vanilla Deluxe (Французкая ваниль (Делюкс))' },</v>
+      </c>
+      <c r="L77" t="str">
+        <f>CONCATENATE($F$1,$G$1,C77,$H$1,C77,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>293</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Frosted Donut (Пончик)', </v>
+        <v>'Frosted Donut (Пончик)'</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Frosted Donut (Пончик)', name: 'Frosted Donut (Пончик)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
+        <v>{name: 'Frosted Donut (Пончик)' },</v>
+      </c>
+      <c r="L78" t="str">
+        <f>CONCATENATE($F$1,$G$1,C78,$H$1,C78,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>294</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Fruit Circles (Фруктовые кольца)', </v>
+        <v>'Fruit Circles (Фруктовые кольца)'</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Fruit Circles (Фруктовые кольца)', name: 'Fruit Circles (Фруктовые кольца)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11">
+        <v>{name: 'Fruit Circles (Фруктовые кольца)' },</v>
+      </c>
+      <c r="L79" t="str">
+        <f>CONCATENATE($F$1,$G$1,C79,$H$1,C79,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>295</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Fruit Circles With Milk (Фруктовые кольца с молоком)', </v>
+        <v>'Fruit Circles With Milk (Фруктовые кольца с молоком)'</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Fruit Circles With Milk (Фруктовые кольца с молоком)', name: 'Fruit Circles With Milk (Фруктовые кольца с молоком)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11">
+        <v>{name: 'Fruit Circles With Milk (Фруктовые кольца с молоком)' },</v>
+      </c>
+      <c r="L80" t="str">
+        <f>CONCATENATE($F$1,$G$1,C80,$H$1,C80,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>296</v>
       </c>
       <c r="B81" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Fruity Stick Gum (Жвачка (Fruity Stick))', </v>
+        <v>'Fruity Stick Gum (Жвачка (Fruity Stick))'</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Fruity Stick Gum (Жвачка (Fruity Stick))', name: 'Fruity Stick Gum (Жвачка (Fruity Stick))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11">
+        <v>{name: 'Fruity Stick Gum (Жвачка (Fruity Stick))' },</v>
+      </c>
+      <c r="L81" t="str">
+        <f>CONCATENATE($F$1,$G$1,C81,$H$1,C81,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>297</v>
       </c>
       <c r="B82" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Fudge Brownie (Брауни)', </v>
+        <v>'Fudge Brownie (Брауни)'</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Fudge Brownie (Брауни)', name: 'Fudge Brownie (Брауни)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11">
+        <v>{name: 'Fudge Brownie (Брауни)' },</v>
+      </c>
+      <c r="L82" t="str">
+        <f>CONCATENATE($F$1,$G$1,C82,$H$1,C82,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>298</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Ginger Ale (Имбирный Эль)', </v>
+        <v>'Ginger Ale (Имбирный Эль)'</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Ginger Ale (Имбирный Эль)', name: 'Ginger Ale (Имбирный Эль)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11">
+        <v>{name: 'Ginger Ale (Имбирный Эль)' },</v>
+      </c>
+      <c r="L83" t="str">
+        <f>CONCATENATE($F$1,$G$1,C83,$H$1,C83,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>299</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Gingerbread (Имбирный пряник)', </v>
+        <v>'Gingerbread (Имбирный пряник)'</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Gingerbread (Имбирный пряник)', name: 'Gingerbread (Имбирный пряник)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11">
+        <v>{name: 'Gingerbread (Имбирный пряник)' },</v>
+      </c>
+      <c r="L84" t="str">
+        <f>CONCATENATE($F$1,$G$1,C84,$H$1,C84,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>300</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Graham Cracker (Грэхем крекер)', </v>
+        <v>'Graham Cracker (Грэхем крекер)'</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Graham Cracker (Грэхем крекер)', name: 'Graham Cracker (Грэхем крекер)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11">
+        <v>{name: 'Graham Cracker (Грэхем крекер)' },</v>
+      </c>
+      <c r="L85" t="str">
+        <f>CONCATENATE($F$1,$G$1,C85,$H$1,C85,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>301</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Graham Cracker Clear (Грэхем крекер)', </v>
+        <v>'Graham Cracker Clear (Грэхем крекер)'</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Graham Cracker Clear (Грэхем крекер)', name: 'Graham Cracker Clear (Грэхем крекер)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11">
+        <v>{name: 'Graham Cracker Clear (Грэхем крекер)' },</v>
+      </c>
+      <c r="L86" t="str">
+        <f>CONCATENATE($F$1,$G$1,C86,$H$1,C86,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>302</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Grape Candy (Виноградные леденцы)', </v>
+        <v>'Grape Candy (Виноградные леденцы)'</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Grape Candy (Виноградные леденцы)', name: 'Grape Candy (Виноградные леденцы)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11">
+        <v>{name: 'Grape Candy (Виноградные леденцы)' },</v>
+      </c>
+      <c r="L87" t="str">
+        <f>CONCATENATE($F$1,$G$1,C87,$H$1,C87,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>303</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Grape Juice (Виноградный сок)', </v>
+        <v>'Grape Juice (Виноградный сок)'</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Grape Juice (Виноградный сок)', name: 'Grape Juice (Виноградный сок)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11">
+        <v>{name: 'Grape Juice (Виноградный сок)' },</v>
+      </c>
+      <c r="L88" t="str">
+        <f>CONCATENATE($F$1,$G$1,C88,$H$1,C88,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>304</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Greek Yogurt (Греческий йогурт)', </v>
+        <v>'Greek Yogurt (Греческий йогурт)'</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Greek Yogurt (Греческий йогурт)', name: 'Greek Yogurt (Греческий йогурт)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11">
+        <v>{name: 'Greek Yogurt (Греческий йогурт)' },</v>
+      </c>
+      <c r="L89" t="str">
+        <f>CONCATENATE($F$1,$G$1,C89,$H$1,C89,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>305</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Green Apple (Зеленое яблоко)', </v>
+        <v>'Green Apple (Зеленое яблоко)'</v>
       </c>
       <c r="K90" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Green Apple (Зеленое яблоко)', name: 'Green Apple (Зеленое яблоко)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11">
+        <v>{name: 'Green Apple (Зеленое яблоко)' },</v>
+      </c>
+      <c r="L90" t="str">
+        <f>CONCATENATE($F$1,$G$1,C90,$H$1,C90,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>306</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Green Tea (Зеленый чай)', </v>
+        <v>'Green Tea (Зеленый чай)'</v>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Green Tea (Зеленый чай)', name: 'Green Tea (Зеленый чай)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11">
+        <v>{name: 'Green Tea (Зеленый чай)' },</v>
+      </c>
+      <c r="L91" t="str">
+        <f>CONCATENATE($F$1,$G$1,C91,$H$1,C91,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>307</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Guava (Гуайява)', </v>
+        <v>'Guava (Гуайява)'</v>
       </c>
       <c r="K92" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Guava (Гуайява)', name: 'Guava (Гуайява)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11">
+        <v>{name: 'Guava (Гуайява)' },</v>
+      </c>
+      <c r="L92" t="str">
+        <f>CONCATENATE($F$1,$G$1,C92,$H$1,C92,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>308</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Gummy Candy (Тянучки)', </v>
+        <v>'Gummy Candy (Тянучки)'</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Gummy Candy (Тянучки)', name: 'Gummy Candy (Тянучки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11">
+        <v>{name: 'Gummy Candy (Тянучки)' },</v>
+      </c>
+      <c r="L93" t="str">
+        <f>CONCATENATE($F$1,$G$1,C93,$H$1,C93,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>309</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Hazelnut (Лесной орех)', </v>
+        <v>'Hazelnut (Лесной орех)'</v>
       </c>
       <c r="K94" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Hazelnut (Лесной орех)', name: 'Hazelnut (Лесной орех)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11">
+        <v>{name: 'Hazelnut (Лесной орех)' },</v>
+      </c>
+      <c r="L94" t="str">
+        <f>CONCATENATE($F$1,$G$1,C94,$H$1,C94,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>310</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Hibiscus (Гибискус)', </v>
+        <v>'Hibiscus (Гибискус)'</v>
       </c>
       <c r="K95" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Hibiscus (Гибискус)', name: 'Hibiscus (Гибискус)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11">
+        <v>{name: 'Hibiscus (Гибискус)' },</v>
+      </c>
+      <c r="L95" t="str">
+        <f>CONCATENATE($F$1,$G$1,C95,$H$1,C95,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>311</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Honey (Мед)', </v>
+        <v>'Honey (Мед)'</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Honey (Мед)', name: 'Honey (Мед)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11">
+        <v>{name: 'Honey (Мед)' },</v>
+      </c>
+      <c r="L96" t="str">
+        <f>CONCATENATE($F$1,$G$1,C96,$H$1,C96,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>312</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Honeydew (Медовая дыня)', </v>
+        <v>'Honeydew (Медовая дыня)'</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Honeydew (Медовая дыня)', name: 'Honeydew (Медовая дыня)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
+        <v>{name: 'Honeydew (Медовая дыня)' },</v>
+      </c>
+      <c r="L97" t="str">
+        <f>CONCATENATE($F$1,$G$1,C97,$H$1,C97,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>313</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Honeydew II (Медовая дыня (версия 2))', </v>
+        <v>'Honeydew II (Медовая дыня (версия 2))'</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Honeydew II (Медовая дыня (версия 2))', name: 'Honeydew II (Медовая дыня (версия 2))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
+        <v>{name: 'Honeydew II (Медовая дыня (версия 2))' },</v>
+      </c>
+      <c r="L98" t="str">
+        <f>CONCATENATE($F$1,$G$1,C98,$H$1,C98,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>314</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Honeysuckle (Жимолость)', </v>
+        <v>'Honeysuckle (Жимолость)'</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Honeysuckle (Жимолость)', name: 'Honeysuckle (Жимолость)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11">
+        <v>{name: 'Honeysuckle (Жимолость)' },</v>
+      </c>
+      <c r="L99" t="str">
+        <f>CONCATENATE($F$1,$G$1,C99,$H$1,C99,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>315</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Horehound (Шандра)', </v>
+        <v>'Horehound (Шандра)'</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Horehound (Шандра)', name: 'Horehound (Шандра)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
+        <v>{name: 'Horehound (Шандра)' },</v>
+      </c>
+      <c r="L100" t="str">
+        <f>CONCATENATE($F$1,$G$1,C100,$H$1,C100,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>316</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Huckleberry (Хаклберри)', </v>
+        <v>'Huckleberry (Хаклберри)'</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Huckleberry (Хаклберри)', name: 'Huckleberry (Хаклберри)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11">
+        <v>{name: 'Huckleberry (Хаклберри)' },</v>
+      </c>
+      <c r="L101" t="str">
+        <f>CONCATENATE($F$1,$G$1,C101,$H$1,C101,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>317</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Irish Cream (Ирландские сливки)', </v>
+        <v>'Irish Cream (Ирландские сливки)'</v>
       </c>
       <c r="K102" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Irish Cream (Ирландские сливки)', name: 'Irish Cream (Ирландские сливки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11">
+        <v>{name: 'Irish Cream (Ирландские сливки)' },</v>
+      </c>
+      <c r="L102" t="str">
+        <f>CONCATENATE($F$1,$G$1,C102,$H$1,C102,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>318</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Jackfruit (Джекфрут)', </v>
+        <v>'Jackfruit (Джекфрут)'</v>
       </c>
       <c r="K103" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Jackfruit (Джекфрут)', name: 'Jackfruit (Джекфрут)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11">
+        <v>{name: 'Jackfruit (Джекфрут)' },</v>
+      </c>
+      <c r="L103" t="str">
+        <f>CONCATENATE($F$1,$G$1,C103,$H$1,C103,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>319</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Jamaican Rum (Ямайский ром)', </v>
+        <v>'Jamaican Rum (Ямайский ром)'</v>
       </c>
       <c r="K104" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Jamaican Rum (Ямайский ром)', name: 'Jamaican Rum (Ямайский ром)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11">
+        <v>{name: 'Jamaican Rum (Ямайский ром)' },</v>
+      </c>
+      <c r="L104" t="str">
+        <f>CONCATENATE($F$1,$G$1,C104,$H$1,C104,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>320</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Kalua and Cream (Калуа и сливки)', </v>
+        <v>'Kalua and Cream (Калуа и сливки)'</v>
       </c>
       <c r="K105" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Kalua and Cream (Калуа и сливки)', name: 'Kalua and Cream (Калуа и сливки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11">
+        <v>{name: 'Kalua and Cream (Калуа и сливки)' },</v>
+      </c>
+      <c r="L105" t="str">
+        <f>CONCATENATE($F$1,$G$1,C105,$H$1,C105,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>321</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Kentucky Bourbon (Бурбон из Кентукки)', </v>
+        <v>'Kentucky Bourbon (Бурбон из Кентукки)'</v>
       </c>
       <c r="K106" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Kentucky Bourbon (Бурбон из Кентукки)', name: 'Kentucky Bourbon (Бурбон из Кентукки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11">
+        <v>{name: 'Kentucky Bourbon (Бурбон из Кентукки)' },</v>
+      </c>
+      <c r="L106" t="str">
+        <f>CONCATENATE($F$1,$G$1,C106,$H$1,C106,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>322</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Key Lime (Лайм)', </v>
+        <v>'Key Lime (Лайм)'</v>
       </c>
       <c r="K107" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Key Lime (Лайм)', name: 'Key Lime (Лайм)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11">
+        <v>{name: 'Key Lime (Лайм)' },</v>
+      </c>
+      <c r="L107" t="str">
+        <f>CONCATENATE($F$1,$G$1,C107,$H$1,C107,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>323</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Kiwi (Киви)', </v>
+        <v>'Kiwi (Киви)'</v>
       </c>
       <c r="K108" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Kiwi (Киви)', name: 'Kiwi (Киви)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11">
+        <v>{name: 'Kiwi (Киви)' },</v>
+      </c>
+      <c r="L108" t="str">
+        <f>CONCATENATE($F$1,$G$1,C108,$H$1,C108,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>324</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Kiwi (Double) (Киви (двойной))', </v>
+        <v>'Kiwi (Double) (Киви (двойной))'</v>
       </c>
       <c r="K109" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Kiwi (Double) (Киви (двойной))', name: 'Kiwi (Double) (Киви (двойной))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11">
+        <v>{name: 'Kiwi (Double) (Киви (двойной))' },</v>
+      </c>
+      <c r="L109" t="str">
+        <f>CONCATENATE($F$1,$G$1,C109,$H$1,C109,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>325</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Koolada 10 PG (Кулада)', </v>
+        <v>'Koolada 10 PG (Кулада)'</v>
       </c>
       <c r="K110" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Koolada 10 PG (Кулада)', name: 'Koolada 10 PG (Кулада)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11">
+        <v>{name: 'Koolada 10 PG (Кулада)' },</v>
+      </c>
+      <c r="L110" t="str">
+        <f>CONCATENATE($F$1,$G$1,C110,$H$1,C110,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>326</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lemon (water soluble) (Лимон)', </v>
+        <v>'Lemon (water soluble) (Лимон)'</v>
       </c>
       <c r="K111" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lemon (water soluble) (Лимон)', name: 'Lemon (water soluble) (Лимон)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11">
+        <v>{name: 'Lemon (water soluble) (Лимон)' },</v>
+      </c>
+      <c r="L111" t="str">
+        <f>CONCATENATE($F$1,$G$1,C111,$H$1,C111,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>327</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lemon 2 (Лимон (Версия 2))', </v>
+        <v>'Lemon 2 (Лимон (Версия 2))'</v>
       </c>
       <c r="K112" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lemon 2 (Лимон (Версия 2))', name: 'Lemon 2 (Лимон (Версия 2))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11">
+        <v>{name: 'Lemon 2 (Лимон (Версия 2))' },</v>
+      </c>
+      <c r="L112" t="str">
+        <f>CONCATENATE($F$1,$G$1,C112,$H$1,C112,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>328</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lemon Lime (Лимон-лайм)', </v>
+        <v>'Lemon Lime (Лимон-лайм)'</v>
       </c>
       <c r="K113" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lemon Lime (Лимон-лайм)', name: 'Lemon Lime (Лимон-лайм)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11">
+        <v>{name: 'Lemon Lime (Лимон-лайм)' },</v>
+      </c>
+      <c r="L113" t="str">
+        <f>CONCATENATE($F$1,$G$1,C113,$H$1,C113,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>329</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lemon Lime 2 (Лимон лайм (версия 2))', </v>
+        <v>'Lemon Lime 2 (Лимон лайм (версия 2))'</v>
       </c>
       <c r="K114" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lemon Lime 2 (Лимон лайм (версия 2))', name: 'Lemon Lime 2 (Лимон лайм (версия 2))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11">
+        <v>{name: 'Lemon Lime 2 (Лимон лайм (версия 2))' },</v>
+      </c>
+      <c r="L114" t="str">
+        <f>CONCATENATE($F$1,$G$1,C114,$H$1,C114,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>330</v>
       </c>
       <c r="B115" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lemonade Cookie (Лимонадное печенье)', </v>
+        <v>'Lemonade Cookie (Лимонадное печенье)'</v>
       </c>
       <c r="K115" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lemonade Cookie (Лимонадное печенье)', name: 'Lemonade Cookie (Лимонадное печенье)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11">
+        <v>{name: 'Lemonade Cookie (Лимонадное печенье)' },</v>
+      </c>
+      <c r="L115" t="str">
+        <f>CONCATENATE($F$1,$G$1,C115,$H$1,C115,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>127</v>
       </c>
       <c r="B116" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lucky Leprechaun Cereal (Зефирные хлопья)', </v>
+        <v>'Lucky Leprechaun Cereal (Зефирные хлопья)'</v>
       </c>
       <c r="K116" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lucky Leprechaun Cereal (Зефирные хлопья)', name: 'Lucky Leprechaun Cereal (Зефирные хлопья)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11">
+        <v>{name: 'Lucky Leprechaun Cereal (Зефирные хлопья)' },</v>
+      </c>
+      <c r="L116" t="str">
+        <f>CONCATENATE($F$1,$G$1,C116,$H$1,C116,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>331</v>
       </c>
       <c r="B117" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Lychee (Личи)', </v>
+        <v>'Lychee (Личи)'</v>
       </c>
       <c r="K117" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Lychee (Личи)', name: 'Lychee (Личи)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11">
+        <v>{name: 'Lychee (Личи)' },</v>
+      </c>
+      <c r="L117" t="str">
+        <f>CONCATENATE($F$1,$G$1,C117,$H$1,C117,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>332</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'M Type Premium (Эм тайп премиум (табак))', </v>
+        <v>'M Type Premium (Эм тайп премиум (табак))'</v>
       </c>
       <c r="K118" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'M Type Premium (Эм тайп премиум (табак))', name: 'M Type Premium (Эм тайп премиум (табак))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11">
+        <v>{name: 'M Type Premium (Эм тайп премиум (табак))' },</v>
+      </c>
+      <c r="L118" t="str">
+        <f>CONCATENATE($F$1,$G$1,C118,$H$1,C118,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>333</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Malted milk (Сухое молоко)', </v>
+        <v>'Malted milk (Сухое молоко)'</v>
       </c>
       <c r="K119" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Malted milk (Сухое молоко)', name: 'Malted milk (Сухое молоко)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11">
+        <v>{name: 'Malted milk (Сухое молоко)' },</v>
+      </c>
+      <c r="L119" t="str">
+        <f>CONCATENATE($F$1,$G$1,C119,$H$1,C119,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>334</v>
       </c>
       <c r="B120" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Mango (Манго)', </v>
+        <v>'Mango (Манго)'</v>
       </c>
       <c r="K120" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Mango (Манго)', name: 'Mango (Манго)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11">
+        <v>{name: 'Mango (Манго)' },</v>
+      </c>
+      <c r="L120" t="str">
+        <f>CONCATENATE($F$1,$G$1,C120,$H$1,C120,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>335</v>
       </c>
       <c r="B121" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Maple Extract (Кленовый экстракт)', </v>
+        <v>'Maple Extract (Кленовый экстракт)'</v>
       </c>
       <c r="K121" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Maple Extract (Кленовый экстракт)', name: 'Maple Extract (Кленовый экстракт)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11">
+        <v>{name: 'Maple Extract (Кленовый экстракт)' },</v>
+      </c>
+      <c r="L121" t="str">
+        <f>CONCATENATE($F$1,$G$1,C121,$H$1,C121,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>336</v>
       </c>
       <c r="B122" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Maple Syrup (Кленовый сироп)', </v>
+        <v>'Maple Syrup (Кленовый сироп)'</v>
       </c>
       <c r="K122" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Maple Syrup (Кленовый сироп)', name: 'Maple Syrup (Кленовый сироп)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11">
+        <v>{name: 'Maple Syrup (Кленовый сироп)' },</v>
+      </c>
+      <c r="L122" t="str">
+        <f>CONCATENATE($F$1,$G$1,C122,$H$1,C122,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>337</v>
       </c>
       <c r="B123" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Marshmallow (Маршмеллоу)', </v>
+        <v>'Marshmallow (Маршмеллоу)'</v>
       </c>
       <c r="K123" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Marshmallow (Маршмеллоу)', name: 'Marshmallow (Маршмеллоу)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11">
+        <v>{name: 'Marshmallow (Маршмеллоу)' },</v>
+      </c>
+      <c r="L123" t="str">
+        <f>CONCATENATE($F$1,$G$1,C123,$H$1,C123,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>338</v>
       </c>
       <c r="B124" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Mary Jane (Мери Джейн)', </v>
+        <v>'Mary Jane (Мери Джейн)'</v>
       </c>
       <c r="K124" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Mary Jane (Мери Джейн)', name: 'Mary Jane (Мери Джейн)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11">
+        <v>{name: 'Mary Jane (Мери Джейн)' },</v>
+      </c>
+      <c r="L124" t="str">
+        <f>CONCATENATE($F$1,$G$1,C124,$H$1,C124,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>339</v>
       </c>
       <c r="B125" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Menthol liquid (Ментол)', </v>
+        <v>'Menthol liquid (Ментол)'</v>
       </c>
       <c r="K125" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Menthol liquid (Ментол)', name: 'Menthol liquid (Ментол)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11">
+        <v>{name: 'Menthol liquid (Ментол)' },</v>
+      </c>
+      <c r="L125" t="str">
+        <f>CONCATENATE($F$1,$G$1,C125,$H$1,C125,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>340</v>
       </c>
       <c r="B126" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Meringue (Безе)', </v>
+        <v>'Meringue (Безе)'</v>
       </c>
       <c r="K126" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Meringue (Безе)', name: 'Meringue (Безе)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11">
+        <v>{name: 'Meringue (Безе)' },</v>
+      </c>
+      <c r="L126" t="str">
+        <f>CONCATENATE($F$1,$G$1,C126,$H$1,C126,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>341</v>
       </c>
       <c r="B127" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Milk Chocolate (Молочный шоколад)', </v>
+        <v>'Milk Chocolate (Молочный шоколад)'</v>
       </c>
       <c r="K127" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Milk Chocolate (Молочный шоколад)', name: 'Milk Chocolate (Молочный шоколад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11">
+        <v>{name: 'Milk Chocolate (Молочный шоколад)' },</v>
+      </c>
+      <c r="L127" t="str">
+        <f>CONCATENATE($F$1,$G$1,C127,$H$1,C127,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>342</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Mojito Havana (Мохито)', </v>
+        <v>'Mojito Havana (Мохито)'</v>
       </c>
       <c r="K128" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Mojito Havana (Мохито)', name: 'Mojito Havana (Мохито)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11">
+        <v>{name: 'Mojito Havana (Мохито)' },</v>
+      </c>
+      <c r="L128" t="str">
+        <f>CONCATENATE($F$1,$G$1,C128,$H$1,C128,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" t="s">
         <v>343</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">'Molasses (Меласса)', </v>
+        <v>'Molasses (Меласса)'</v>
       </c>
       <c r="K129" t="str">
         <f t="shared" si="3"/>
-        <v>{id: 'Molasses (Меласса)', name: 'Molasses (Меласса)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11">
+        <v>{name: 'Molasses (Меласса)' },</v>
+      </c>
+      <c r="L129" t="str">
+        <f>CONCATENATE($F$1,$G$1,C129,$H$1,C129,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" t="s">
         <v>344</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" ref="B130:B193" si="4">CONCATENATE("'",A130,"', ")</f>
-        <v xml:space="preserve">'Musk Candy (Конфеты Musk Lifesaver)', </v>
+        <f t="shared" ref="B130:B193" si="4">CONCATENATE("'",A130,"'")</f>
+        <v>'Musk Candy (Конфеты Musk Lifesaver)'</v>
       </c>
       <c r="K130" t="str">
-        <f t="shared" ref="K130:K193" si="5">CONCATENATE($F$1,$G$1,B130,$H$1,B130,$I$1)</f>
-        <v>{id: 'Musk Candy (Конфеты Musk Lifesaver)', name: 'Musk Candy (Конфеты Musk Lifesaver)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11">
+        <f t="shared" ref="K130:K193" si="5">CONCATENATE($F$1,$H$1,B130,$J$1)</f>
+        <v>{name: 'Musk Candy (Конфеты Musk Lifesaver)' },</v>
+      </c>
+      <c r="L130" t="str">
+        <f>CONCATENATE($F$1,$G$1,C130,$H$1,C130,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" t="s">
         <v>345</v>
       </c>
       <c r="B131" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Nectarine (Нектарин)', </v>
+        <v>'Nectarine (Нектарин)'</v>
       </c>
       <c r="K131" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Nectarine (Нектарин)', name: 'Nectarine (Нектарин)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11">
+        <v>{name: 'Nectarine (Нектарин)' },</v>
+      </c>
+      <c r="L131" t="str">
+        <f>CONCATENATE($F$1,$G$1,C131,$H$1,C131,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" t="s">
         <v>346</v>
       </c>
       <c r="B132" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Oatmeal Cookie (Овсянное печенье)', </v>
+        <v>'Oatmeal Cookie (Овсянное печенье)'</v>
       </c>
       <c r="K132" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Oatmeal Cookie (Овсянное печенье)', name: 'Oatmeal Cookie (Овсянное печенье)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11">
+        <v>{name: 'Oatmeal Cookie (Овсянное печенье)' },</v>
+      </c>
+      <c r="L132" t="str">
+        <f>CONCATENATE($F$1,$G$1,C132,$H$1,C132,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" t="s">
         <v>347</v>
       </c>
       <c r="B133" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Orange Cream (Апельсиновый крем)', </v>
+        <v>'Orange Cream (Апельсиновый крем)'</v>
       </c>
       <c r="K133" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Orange Cream (Апельсиновый крем)', name: 'Orange Cream (Апельсиновый крем)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11">
+        <v>{name: 'Orange Cream (Апельсиновый крем)' },</v>
+      </c>
+      <c r="L133" t="str">
+        <f>CONCATENATE($F$1,$G$1,C133,$H$1,C133,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" t="s">
         <v>348</v>
       </c>
       <c r="B134" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Orange Mandarin (Мандарин)', </v>
+        <v>'Orange Mandarin (Мандарин)'</v>
       </c>
       <c r="K134" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Orange Mandarin (Мандарин)', name: 'Orange Mandarin (Мандарин)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11">
+        <v>{name: 'Orange Mandarin (Мандарин)' },</v>
+      </c>
+      <c r="L134" t="str">
+        <f>CONCATENATE($F$1,$G$1,C134,$H$1,C134,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" t="s">
         <v>349</v>
       </c>
       <c r="B135" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pancake (Панкейк)', </v>
+        <v>'Pancake (Панкейк)'</v>
       </c>
       <c r="K135" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pancake (Панкейк)', name: 'Pancake (Панкейк)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11">
+        <v>{name: 'Pancake (Панкейк)' },</v>
+      </c>
+      <c r="L135" t="str">
+        <f>CONCATENATE($F$1,$G$1,C135,$H$1,C135,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>350</v>
       </c>
       <c r="B136" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Papaya (Папайя)', </v>
+        <v>'Papaya (Папайя)'</v>
       </c>
       <c r="K136" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Papaya (Папайя)', name: 'Papaya (Папайя)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11">
+        <v>{name: 'Papaya (Папайя)' },</v>
+      </c>
+      <c r="L136" t="str">
+        <f>CONCATENATE($F$1,$G$1,C136,$H$1,C136,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>351</v>
       </c>
       <c r="B137" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Passion Fruit (Маракуйя)', </v>
+        <v>'Passion Fruit (Маракуйя)'</v>
       </c>
       <c r="K137" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Passion Fruit (Маракуйя)', name: 'Passion Fruit (Маракуйя)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11">
+        <v>{name: 'Passion Fruit (Маракуйя)' },</v>
+      </c>
+      <c r="L137" t="str">
+        <f>CONCATENATE($F$1,$G$1,C137,$H$1,C137,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" t="s">
         <v>352</v>
       </c>
       <c r="B138" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Peach (Персик)', </v>
+        <v>'Peach (Персик)'</v>
       </c>
       <c r="K138" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Peach (Персик)', name: 'Peach (Персик)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11">
+        <v>{name: 'Peach (Персик)' },</v>
+      </c>
+      <c r="L138" t="str">
+        <f>CONCATENATE($F$1,$G$1,C138,$H$1,C138,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>353</v>
       </c>
       <c r="B139" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Peach (Juicy) (Сок персика)', </v>
+        <v>'Peach (Juicy) (Сок персика)'</v>
       </c>
       <c r="K139" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Peach (Juicy) (Сок персика)', name: 'Peach (Juicy) (Сок персика)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11">
+        <v>{name: 'Peach (Juicy) (Сок персика)' },</v>
+      </c>
+      <c r="L139" t="str">
+        <f>CONCATENATE($F$1,$G$1,C139,$H$1,C139,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>354</v>
       </c>
       <c r="B140" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Peanut Butter (Арахисовое масло)', </v>
+        <v>'Peanut Butter (Арахисовое масло)'</v>
       </c>
       <c r="K140" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Peanut Butter (Арахисовое масло)', name: 'Peanut Butter (Арахисовое масло)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11">
+        <v>{name: 'Peanut Butter (Арахисовое масло)' },</v>
+      </c>
+      <c r="L140" t="str">
+        <f>CONCATENATE($F$1,$G$1,C140,$H$1,C140,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="A141" t="s">
         <v>355</v>
       </c>
       <c r="B141" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pear (Груша)', </v>
+        <v>'Pear (Груша)'</v>
       </c>
       <c r="K141" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pear (Груша)', name: 'Pear (Груша)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11">
+        <v>{name: 'Pear (Груша)' },</v>
+      </c>
+      <c r="L141" t="str">
+        <f>CONCATENATE($F$1,$G$1,C141,$H$1,C141,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" t="s">
         <v>356</v>
       </c>
       <c r="B142" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pear Candy (Грушевые конфеты)', </v>
+        <v>'Pear Candy (Грушевые конфеты)'</v>
       </c>
       <c r="K142" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pear Candy (Грушевые конфеты)', name: 'Pear Candy (Грушевые конфеты)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11">
+        <v>{name: 'Pear Candy (Грушевые конфеты)' },</v>
+      </c>
+      <c r="L142" t="str">
+        <f>CONCATENATE($F$1,$G$1,C142,$H$1,C142,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" t="s">
         <v>357</v>
       </c>
       <c r="B143" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pecan (Орех Пекан)', </v>
+        <v>'Pecan (Орех Пекан)'</v>
       </c>
       <c r="K143" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pecan (Орех Пекан)', name: 'Pecan (Орех Пекан)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11">
+        <v>{name: 'Pecan (Орех Пекан)' },</v>
+      </c>
+      <c r="L143" t="str">
+        <f>CONCATENATE($F$1,$G$1,C143,$H$1,C143,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" t="s">
         <v>358</v>
       </c>
       <c r="B144" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Peppermint (Перечная мята)', </v>
+        <v>'Peppermint (Перечная мята)'</v>
       </c>
       <c r="K144" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Peppermint (Перечная мята)', name: 'Peppermint (Перечная мята)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11">
+        <v>{name: 'Peppermint (Перечная мята)' },</v>
+      </c>
+      <c r="L144" t="str">
+        <f>CONCATENATE($F$1,$G$1,C144,$H$1,C144,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
       <c r="A145" t="s">
         <v>359</v>
       </c>
       <c r="B145" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pie Crust (Корочка пирога)', </v>
+        <v>'Pie Crust (Корочка пирога)'</v>
       </c>
       <c r="K145" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pie Crust (Корочка пирога)', name: 'Pie Crust (Корочка пирога)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11">
+        <v>{name: 'Pie Crust (Корочка пирога)' },</v>
+      </c>
+      <c r="L145" t="str">
+        <f>CONCATENATE($F$1,$G$1,C145,$H$1,C145,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
       <c r="A146" t="s">
         <v>161</v>
       </c>
       <c r="B146" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pina Colada (Пина Колада)', </v>
+        <v>'Pina Colada (Пина Колада)'</v>
       </c>
       <c r="K146" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pina Colada (Пина Колада)', name: 'Pina Colada (Пина Колада)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11">
+        <v>{name: 'Pina Colada (Пина Колада)' },</v>
+      </c>
+      <c r="L146" t="str">
+        <f>CONCATENATE($F$1,$G$1,C146,$H$1,C146,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="A147" t="s">
         <v>360</v>
       </c>
       <c r="B147" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pineapple (Ананас)', </v>
+        <v>'Pineapple (Ананас)'</v>
       </c>
       <c r="K147" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pineapple (Ананас)', name: 'Pineapple (Ананас)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11">
+        <v>{name: 'Pineapple (Ананас)' },</v>
+      </c>
+      <c r="L147" t="str">
+        <f>CONCATENATE($F$1,$G$1,C147,$H$1,C147,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" t="s">
         <v>361</v>
       </c>
       <c r="B148" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pistachio (Фисташки)', </v>
+        <v>'Pistachio (Фисташки)'</v>
       </c>
       <c r="K148" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pistachio (Фисташки)', name: 'Pistachio (Фисташки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11">
+        <v>{name: 'Pistachio (Фисташки)' },</v>
+      </c>
+      <c r="L148" t="str">
+        <f>CONCATENATE($F$1,$G$1,C148,$H$1,C148,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
       <c r="A149" t="s">
         <v>362</v>
       </c>
       <c r="B149" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Plum (Слива)', </v>
+        <v>'Plum (Слива)'</v>
       </c>
       <c r="K149" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Plum (Слива)', name: 'Plum (Слива)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11">
+        <v>{name: 'Plum (Слива)' },</v>
+      </c>
+      <c r="L149" t="str">
+        <f>CONCATENATE($F$1,$G$1,C149,$H$1,C149,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
       <c r="A150" t="s">
         <v>363</v>
       </c>
       <c r="B150" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pomegranate (Гранат)', </v>
+        <v>'Pomegranate (Гранат)'</v>
       </c>
       <c r="K150" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pomegranate (Гранат)', name: 'Pomegranate (Гранат)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11">
+        <v>{name: 'Pomegranate (Гранат)' },</v>
+      </c>
+      <c r="L150" t="str">
+        <f>CONCATENATE($F$1,$G$1,C150,$H$1,C150,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
       <c r="A151" t="s">
         <v>364</v>
       </c>
       <c r="B151" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Pomegranate Deluxe (Гранат (делюкс))', </v>
+        <v>'Pomegranate Deluxe (Гранат (делюкс))'</v>
       </c>
       <c r="K151" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Pomegranate Deluxe (Гранат (делюкс))', name: 'Pomegranate Deluxe (Гранат (делюкс))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11">
+        <v>{name: 'Pomegranate Deluxe (Гранат (делюкс))' },</v>
+      </c>
+      <c r="L151" t="str">
+        <f>CONCATENATE($F$1,$G$1,C151,$H$1,C151,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
       <c r="A152" t="s">
         <v>167</v>
       </c>
       <c r="B152" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Popcorn (Попкорн)', </v>
+        <v>'Popcorn (Попкорн)'</v>
       </c>
       <c r="K152" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Popcorn (Попкорн)', name: 'Popcorn (Попкорн)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11">
+        <v>{name: 'Popcorn (Попкорн)' },</v>
+      </c>
+      <c r="L152" t="str">
+        <f>CONCATENATE($F$1,$G$1,C152,$H$1,C152,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
         <v>365</v>
       </c>
       <c r="B153" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Quince (Айва)', </v>
+        <v>'Quince (Айва)'</v>
       </c>
       <c r="K153" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Quince (Айва)', name: 'Quince (Айва)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11">
+        <v>{name: 'Quince (Айва)' },</v>
+      </c>
+      <c r="L153" t="str">
+        <f>CONCATENATE($F$1,$G$1,C153,$H$1,C153,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
       <c r="A154" t="s">
         <v>366</v>
       </c>
       <c r="B154" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Rainbow Drops (Скиттлс)', </v>
+        <v>'Rainbow Drops (Скиттлс)'</v>
       </c>
       <c r="K154" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Rainbow Drops (Скиттлс)', name: 'Rainbow Drops (Скиттлс)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11">
+        <v>{name: 'Rainbow Drops (Скиттлс)' },</v>
+      </c>
+      <c r="L154" t="str">
+        <f>CONCATENATE($F$1,$G$1,C154,$H$1,C154,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
       <c r="A155" t="s">
         <v>367</v>
       </c>
       <c r="B155" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Raisin (Изюм)', </v>
+        <v>'Raisin (Изюм)'</v>
       </c>
       <c r="K155" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Raisin (Изюм)', name: 'Raisin (Изюм)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11">
+        <v>{name: 'Raisin (Изюм)' },</v>
+      </c>
+      <c r="L155" t="str">
+        <f>CONCATENATE($F$1,$G$1,C155,$H$1,C155,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
       <c r="A156" t="s">
         <v>368</v>
       </c>
       <c r="B156" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Raspberry (Малина)', </v>
+        <v>'Raspberry (Малина)'</v>
       </c>
       <c r="K156" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Raspberry (Малина)', name: 'Raspberry (Малина)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11">
+        <v>{name: 'Raspberry (Малина)' },</v>
+      </c>
+      <c r="L156" t="str">
+        <f>CONCATENATE($F$1,$G$1,C156,$H$1,C156,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
       <c r="A157" t="s">
         <v>369</v>
       </c>
       <c r="B157" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Raspberry (Sweet) (Сладкая малина)', </v>
+        <v>'Raspberry (Sweet) (Сладкая малина)'</v>
       </c>
       <c r="K157" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Raspberry (Sweet) (Сладкая малина)', name: 'Raspberry (Sweet) (Сладкая малина)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11">
+        <v>{name: 'Raspberry (Sweet) (Сладкая малина)' },</v>
+      </c>
+      <c r="L157" t="str">
+        <f>CONCATENATE($F$1,$G$1,C157,$H$1,C157,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>370</v>
       </c>
       <c r="B158" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Red Licorice (Красная лакрица)', </v>
+        <v>'Red Licorice (Красная лакрица)'</v>
       </c>
       <c r="K158" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Red Licorice (Красная лакрица)', name: 'Red Licorice (Красная лакрица)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11">
+        <v>{name: 'Red Licorice (Красная лакрица)' },</v>
+      </c>
+      <c r="L158" t="str">
+        <f>CONCATENATE($F$1,$G$1,C158,$H$1,C158,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>371</v>
       </c>
       <c r="B159" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Red Type II Blend (Ред тайп (табак))', </v>
+        <v>'Red Type II Blend (Ред тайп (табак))'</v>
       </c>
       <c r="K159" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Red Type II Blend (Ред тайп (табак))', name: 'Red Type II Blend (Ред тайп (табак))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11">
+        <v>{name: 'Red Type II Blend (Ред тайп (табак))' },</v>
+      </c>
+      <c r="L159" t="str">
+        <f>CONCATENATE($F$1,$G$1,C159,$H$1,C159,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>372</v>
       </c>
       <c r="B160" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Rice Crunchies (Рисовые хлопья)', </v>
+        <v>'Rice Crunchies (Рисовые хлопья)'</v>
       </c>
       <c r="K160" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Rice Crunchies (Рисовые хлопья)', name: 'Rice Crunchies (Рисовые хлопья)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11">
+        <v>{name: 'Rice Crunchies (Рисовые хлопья)' },</v>
+      </c>
+      <c r="L160" t="str">
+        <f>CONCATENATE($F$1,$G$1,C160,$H$1,C160,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>373</v>
       </c>
       <c r="B161" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Ripe Banana (Спелый банан)', </v>
+        <v>'Ripe Banana (Спелый банан)'</v>
       </c>
       <c r="K161" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Ripe Banana (Спелый банан)', name: 'Ripe Banana (Спелый банан)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11">
+        <v>{name: 'Ripe Banana (Спелый банан)' },</v>
+      </c>
+      <c r="L161" t="str">
+        <f>CONCATENATE($F$1,$G$1,C161,$H$1,C161,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>374</v>
       </c>
       <c r="B162" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Root beer flavor (pg) (Рутбир)', </v>
+        <v>'Root beer flavor (pg) (Рутбир)'</v>
       </c>
       <c r="K162" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Root beer flavor (pg) (Рутбир)', name: 'Root beer flavor (pg) (Рутбир)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11">
+        <v>{name: 'Root beer flavor (pg) (Рутбир)' },</v>
+      </c>
+      <c r="L162" t="str">
+        <f>CONCATENATE($F$1,$G$1,C162,$H$1,C162,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>375</v>
       </c>
       <c r="B163" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Root Beer Float (Рутбир Float)', </v>
+        <v>'Root Beer Float (Рутбир Float)'</v>
       </c>
       <c r="K163" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Root Beer Float (Рутбир Float)', name: 'Root Beer Float (Рутбир Float)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11">
+        <v>{name: 'Root Beer Float (Рутбир Float)' },</v>
+      </c>
+      <c r="L163" t="str">
+        <f>CONCATENATE($F$1,$G$1,C163,$H$1,C163,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>376</v>
       </c>
       <c r="B164" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'RY4 Double (RY4 (Табак (двойной)))', </v>
+        <v>'RY4 Double (RY4 (Табак (двойной)))'</v>
       </c>
       <c r="K164" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'RY4 Double (RY4 (Табак (двойной)))', name: 'RY4 Double (RY4 (Табак (двойной)))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11">
+        <v>{name: 'RY4 Double (RY4 (Табак (двойной)))' },</v>
+      </c>
+      <c r="L164" t="str">
+        <f>CONCATENATE($F$1,$G$1,C164,$H$1,C164,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>377</v>
       </c>
       <c r="B165" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'RY4 Type (RY4 (Табак))', </v>
+        <v>'RY4 Type (RY4 (Табак))'</v>
       </c>
       <c r="K165" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'RY4 Type (RY4 (Табак))', name: 'RY4 Type (RY4 (Табак))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11">
+        <v>{name: 'RY4 Type (RY4 (Табак))' },</v>
+      </c>
+      <c r="L165" t="str">
+        <f>CONCATENATE($F$1,$G$1,C165,$H$1,C165,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>378</v>
       </c>
       <c r="B166" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Slim Mint Cookie (Мятное печенье)', </v>
+        <v>'Slim Mint Cookie (Мятное печенье)'</v>
       </c>
       <c r="K166" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Slim Mint Cookie (Мятное печенье)', name: 'Slim Mint Cookie (Мятное печенье)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11">
+        <v>{name: 'Slim Mint Cookie (Мятное печенье)' },</v>
+      </c>
+      <c r="L166" t="str">
+        <f>CONCATENATE($F$1,$G$1,C166,$H$1,C166,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
         <v>379</v>
       </c>
       <c r="B167" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Smooth (Smooth)', </v>
+        <v>'Smooth (Smooth)'</v>
       </c>
       <c r="K167" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Smooth (Smooth)', name: 'Smooth (Smooth)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11">
+        <v>{name: 'Smooth (Smooth)' },</v>
+      </c>
+      <c r="L167" t="str">
+        <f>CONCATENATE($F$1,$G$1,C167,$H$1,C167,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
       <c r="A168" t="s">
         <v>380</v>
       </c>
       <c r="B168" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Sour (Кислый)', </v>
+        <v>'Sour (Кислый)'</v>
       </c>
       <c r="K168" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Sour (Кислый)', name: 'Sour (Кислый)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11">
+        <v>{name: 'Sour (Кислый)' },</v>
+      </c>
+      <c r="L168" t="str">
+        <f>CONCATENATE($F$1,$G$1,C168,$H$1,C168,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
       <c r="A169" t="s">
         <v>381</v>
       </c>
       <c r="B169" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Spearmint (Мята колосистая)', </v>
+        <v>'Spearmint (Мята колосистая)'</v>
       </c>
       <c r="K169" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Spearmint (Мята колосистая)', name: 'Spearmint (Мята колосистая)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11">
+        <v>{name: 'Spearmint (Мята колосистая)' },</v>
+      </c>
+      <c r="L169" t="str">
+        <f>CONCATENATE($F$1,$G$1,C169,$H$1,C169,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
       <c r="A170" t="s">
         <v>382</v>
       </c>
       <c r="B170" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Strawberries and Cream (Клубника со сливками)', </v>
+        <v>'Strawberries and Cream (Клубника со сливками)'</v>
       </c>
       <c r="K170" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Strawberries and Cream (Клубника со сливками)', name: 'Strawberries and Cream (Клубника со сливками)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11">
+        <v>{name: 'Strawberries and Cream (Клубника со сливками)' },</v>
+      </c>
+      <c r="L170" t="str">
+        <f>CONCATENATE($F$1,$G$1,C170,$H$1,C170,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
       <c r="A171" t="s">
         <v>383</v>
       </c>
       <c r="B171" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Strawberry (Клубника)', </v>
+        <v>'Strawberry (Клубника)'</v>
       </c>
       <c r="K171" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Strawberry (Клубника)', name: 'Strawberry (Клубника)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11">
+        <v>{name: 'Strawberry (Клубника)' },</v>
+      </c>
+      <c r="L171" t="str">
+        <f>CONCATENATE($F$1,$G$1,C171,$H$1,C171,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
       <c r="A172" t="s">
         <v>384</v>
       </c>
       <c r="B172" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Strawberry (Ripe) (Спелая клубника)', </v>
+        <v>'Strawberry (Ripe) (Спелая клубника)'</v>
       </c>
       <c r="K172" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Strawberry (Ripe) (Спелая клубника)', name: 'Strawberry (Ripe) (Спелая клубника)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11">
+        <v>{name: 'Strawberry (Ripe) (Спелая клубника)' },</v>
+      </c>
+      <c r="L172" t="str">
+        <f>CONCATENATE($F$1,$G$1,C172,$H$1,C172,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
       <c r="A173" t="s">
         <v>385</v>
       </c>
       <c r="B173" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Swedish Gummy (Шведский гамми)', </v>
+        <v>'Swedish Gummy (Шведский гамми)'</v>
       </c>
       <c r="K173" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Swedish Gummy (Шведский гамми)', name: 'Swedish Gummy (Шведский гамми)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11">
+        <v>{name: 'Swedish Gummy (Шведский гамми)' },</v>
+      </c>
+      <c r="L173" t="str">
+        <f>CONCATENATE($F$1,$G$1,C173,$H$1,C173,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
       <c r="A174" t="s">
         <v>386</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Sweet and Tart (Кофеты Sweet Tart (Холодок))', </v>
+        <v>'Sweet and Tart (Кофеты Sweet Tart (Холодок))'</v>
       </c>
       <c r="K174" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Sweet and Tart (Кофеты Sweet Tart (Холодок))', name: 'Sweet and Tart (Кофеты Sweet Tart (Холодок))', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11">
+        <v>{name: 'Sweet and Tart (Кофеты Sweet Tart (Холодок))' },</v>
+      </c>
+      <c r="L174" t="str">
+        <f>CONCATENATE($F$1,$G$1,C174,$H$1,C174,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>387</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Sweet Cream (Сладкий крем)', </v>
+        <v>'Sweet Cream (Сладкий крем)'</v>
       </c>
       <c r="K175" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Sweet Cream (Сладкий крем)', name: 'Sweet Cream (Сладкий крем)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11">
+        <v>{name: 'Sweet Cream (Сладкий крем)' },</v>
+      </c>
+      <c r="L175" t="str">
+        <f>CONCATENATE($F$1,$G$1,C175,$H$1,C175,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>388</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Sweet Tea (Сладкий чай)', </v>
+        <v>'Sweet Tea (Сладкий чай)'</v>
       </c>
       <c r="K176" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Sweet Tea (Сладкий чай)', name: 'Sweet Tea (Сладкий чай)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11">
+        <v>{name: 'Sweet Tea (Сладкий чай)' },</v>
+      </c>
+      <c r="L176" t="str">
+        <f>CONCATENATE($F$1,$G$1,C176,$H$1,C176,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>389</v>
       </c>
       <c r="B177" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Sweetener (Подсластитель)', </v>
+        <v>'Sweetener (Подсластитель)'</v>
       </c>
       <c r="K177" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Sweetener (Подсластитель)', name: 'Sweetener (Подсластитель)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11">
+        <v>{name: 'Sweetener (Подсластитель)' },</v>
+      </c>
+      <c r="L177" t="str">
+        <f>CONCATENATE($F$1,$G$1,C177,$H$1,C177,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
       <c r="A178" t="s">
         <v>390</v>
       </c>
       <c r="B178" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Tiramisu (Тирамису)', </v>
+        <v>'Tiramisu (Тирамису)'</v>
       </c>
       <c r="K178" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Tiramisu (Тирамису)', name: 'Tiramisu (Тирамису)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11">
+        <v>{name: 'Tiramisu (Тирамису)' },</v>
+      </c>
+      <c r="L178" t="str">
+        <f>CONCATENATE($F$1,$G$1,C178,$H$1,C178,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="A179" t="s">
         <v>391</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Toasted Almond (Жаренный миндаль)', </v>
+        <v>'Toasted Almond (Жаренный миндаль)'</v>
       </c>
       <c r="K179" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Toasted Almond (Жаренный миндаль)', name: 'Toasted Almond (Жаренный миндаль)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11">
+        <v>{name: 'Toasted Almond (Жаренный миндаль)' },</v>
+      </c>
+      <c r="L179" t="str">
+        <f>CONCATENATE($F$1,$G$1,C179,$H$1,C179,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
       <c r="A180" t="s">
         <v>392</v>
       </c>
       <c r="B180" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Toasted Marshmallow (Поджареный зефир)', </v>
+        <v>'Toasted Marshmallow (Поджареный зефир)'</v>
       </c>
       <c r="K180" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Toasted Marshmallow (Поджареный зефир)', name: 'Toasted Marshmallow (Поджареный зефир)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11">
+        <v>{name: 'Toasted Marshmallow (Поджареный зефир)' },</v>
+      </c>
+      <c r="L180" t="str">
+        <f>CONCATENATE($F$1,$G$1,C180,$H$1,C180,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
       <c r="A181" t="s">
         <v>393</v>
       </c>
       <c r="B181" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Tutti-Frutti (Тутти-фрутти)', </v>
+        <v>'Tutti-Frutti (Тутти-фрутти)'</v>
       </c>
       <c r="K181" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Tutti-Frutti (Тутти-фрутти)', name: 'Tutti-Frutti (Тутти-фрутти)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11">
+        <v>{name: 'Tutti-Frutti (Тутти-фрутти)' },</v>
+      </c>
+      <c r="L181" t="str">
+        <f>CONCATENATE($F$1,$G$1,C181,$H$1,C181,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
       <c r="A182" t="s">
         <v>394</v>
       </c>
       <c r="B182" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla (Bourbon) (Ваниль бурбон)', </v>
+        <v>'Vanilla (Bourbon) (Ваниль бурбон)'</v>
       </c>
       <c r="K182" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla (Bourbon) (Ваниль бурбон)', name: 'Vanilla (Bourbon) (Ваниль бурбон)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11">
+        <v>{name: 'Vanilla (Bourbon) (Ваниль бурбон)' },</v>
+      </c>
+      <c r="L182" t="str">
+        <f>CONCATENATE($F$1,$G$1,C182,$H$1,C182,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
       <c r="A183" t="s">
         <v>395</v>
       </c>
       <c r="B183" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla Bean Gelato (Ванильный заварной крем)', </v>
+        <v>'Vanilla Bean Gelato (Ванильный заварной крем)'</v>
       </c>
       <c r="K183" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla Bean Gelato (Ванильный заварной крем)', name: 'Vanilla Bean Gelato (Ванильный заварной крем)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11">
+        <v>{name: 'Vanilla Bean Gelato (Ванильный заварной крем)' },</v>
+      </c>
+      <c r="L183" t="str">
+        <f>CONCATENATE($F$1,$G$1,C183,$H$1,C183,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12">
       <c r="A184" t="s">
         <v>396</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla Bean Ice Cream (Ванильное мороженное)', </v>
+        <v>'Vanilla Bean Ice Cream (Ванильное мороженное)'</v>
       </c>
       <c r="K184" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla Bean Ice Cream (Ванильное мороженное)', name: 'Vanilla Bean Ice Cream (Ванильное мороженное)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11">
+        <v>{name: 'Vanilla Bean Ice Cream (Ванильное мороженное)' },</v>
+      </c>
+      <c r="L184" t="str">
+        <f>CONCATENATE($F$1,$G$1,C184,$H$1,C184,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12">
       <c r="A185" t="s">
         <v>397</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla Cupcake (Ванильный пирог)', </v>
+        <v>'Vanilla Cupcake (Ванильный пирог)'</v>
       </c>
       <c r="K185" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla Cupcake (Ванильный пирог)', name: 'Vanilla Cupcake (Ванильный пирог)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11">
+        <v>{name: 'Vanilla Cupcake (Ванильный пирог)' },</v>
+      </c>
+      <c r="L185" t="str">
+        <f>CONCATENATE($F$1,$G$1,C185,$H$1,C185,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12">
       <c r="A186" t="s">
         <v>398</v>
       </c>
       <c r="B186" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla Custard (Ванильный кастард)', </v>
+        <v>'Vanilla Custard (Ванильный кастард)'</v>
       </c>
       <c r="K186" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla Custard (Ванильный кастард)', name: 'Vanilla Custard (Ванильный кастард)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11">
+        <v>{name: 'Vanilla Custard (Ванильный кастард)' },</v>
+      </c>
+      <c r="L186" t="str">
+        <f>CONCATENATE($F$1,$G$1,C186,$H$1,C186,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12">
       <c r="A187" t="s">
         <v>399</v>
       </c>
       <c r="B187" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanilla Swirl (Ванильный рожок)', </v>
+        <v>'Vanilla Swirl (Ванильный рожок)'</v>
       </c>
       <c r="K187" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanilla Swirl (Ванильный рожок)', name: 'Vanilla Swirl (Ванильный рожок)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11">
+        <v>{name: 'Vanilla Swirl (Ванильный рожок)' },</v>
+      </c>
+      <c r="L187" t="str">
+        <f>CONCATENATE($F$1,$G$1,C187,$H$1,C187,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12">
       <c r="A188" t="s">
         <v>400</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Vanillin 10 (PG) (Ванилин)', </v>
+        <v>'Vanillin 10 (PG) (Ванилин)'</v>
       </c>
       <c r="K188" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Vanillin 10 (PG) (Ванилин)', name: 'Vanillin 10 (PG) (Ванилин)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11">
+        <v>{name: 'Vanillin 10 (PG) (Ванилин)' },</v>
+      </c>
+      <c r="L188" t="str">
+        <f>CONCATENATE($F$1,$G$1,C188,$H$1,C188,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12">
       <c r="A189" t="s">
         <v>401</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Waffle (Вафли)', </v>
+        <v>'Waffle (Вафли)'</v>
       </c>
       <c r="K189" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Waffle (Вафли)', name: 'Waffle (Вафли)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11">
+        <v>{name: 'Waffle (Вафли)' },</v>
+      </c>
+      <c r="L189" t="str">
+        <f>CONCATENATE($F$1,$G$1,C189,$H$1,C189,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
       <c r="A190" t="s">
         <v>211</v>
       </c>
       <c r="B190" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Waffle (Belgian) (Бельгийские вафли)', </v>
+        <v>'Waffle (Belgian) (Бельгийские вафли)'</v>
       </c>
       <c r="K190" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Waffle (Belgian) (Бельгийские вафли)', name: 'Waffle (Belgian) (Бельгийские вафли)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11">
+        <v>{name: 'Waffle (Belgian) (Бельгийские вафли)' },</v>
+      </c>
+      <c r="L190" t="str">
+        <f>CONCATENATE($F$1,$G$1,C190,$H$1,C190,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
       <c r="A191" t="s">
         <v>402</v>
       </c>
       <c r="B191" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Watermelon (Арбуз)', </v>
+        <v>'Watermelon (Арбуз)'</v>
       </c>
       <c r="K191" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Watermelon (Арбуз)', name: 'Watermelon (Арбуз)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11">
+        <v>{name: 'Watermelon (Арбуз)' },</v>
+      </c>
+      <c r="L191" t="str">
+        <f>CONCATENATE($F$1,$G$1,C191,$H$1,C191,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12">
       <c r="A192" t="s">
         <v>403</v>
       </c>
       <c r="B192" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Watermelon Candy (Арбузные леденцы)', </v>
+        <v>'Watermelon Candy (Арбузные леденцы)'</v>
       </c>
       <c r="K192" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Watermelon Candy (Арбузные леденцы)', name: 'Watermelon Candy (Арбузные леденцы)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11">
+        <v>{name: 'Watermelon Candy (Арбузные леденцы)' },</v>
+      </c>
+      <c r="L192" t="str">
+        <f>CONCATENATE($F$1,$G$1,C192,$H$1,C192,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12">
       <c r="A193" t="s">
         <v>404</v>
       </c>
       <c r="B193" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">'Western (Вестерн)', </v>
+        <v>'Western (Вестерн)'</v>
       </c>
       <c r="K193" t="str">
         <f t="shared" si="5"/>
-        <v>{id: 'Western (Вестерн)', name: 'Western (Вестерн)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11">
+        <v>{name: 'Western (Вестерн)' },</v>
+      </c>
+      <c r="L193" t="str">
+        <f>CONCATENATE($F$1,$G$1,C193,$H$1,C193,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12">
       <c r="A194" t="s">
         <v>405</v>
       </c>
       <c r="B194" t="str">
-        <f t="shared" ref="B194:B197" si="6">CONCATENATE("'",A194,"', ")</f>
-        <v xml:space="preserve">'Whipped Cream (Взбитые сливки)', </v>
+        <f t="shared" ref="B194:B197" si="6">CONCATENATE("'",A194,"'")</f>
+        <v>'Whipped Cream (Взбитые сливки)'</v>
       </c>
       <c r="K194" t="str">
-        <f t="shared" ref="K194:K197" si="7">CONCATENATE($F$1,$G$1,B194,$H$1,B194,$I$1)</f>
-        <v>{id: 'Whipped Cream (Взбитые сливки)', name: 'Whipped Cream (Взбитые сливки)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11">
+        <f t="shared" ref="K194:K197" si="7">CONCATENATE($F$1,$H$1,B194,$J$1)</f>
+        <v>{name: 'Whipped Cream (Взбитые сливки)' },</v>
+      </c>
+      <c r="L194" t="str">
+        <f>CONCATENATE($F$1,$G$1,C194,$H$1,C194,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12">
       <c r="A195" t="s">
         <v>406</v>
       </c>
       <c r="B195" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">'White Chocolate (Белый шоколад)', </v>
+        <v>'White Chocolate (Белый шоколад)'</v>
       </c>
       <c r="K195" t="str">
         <f t="shared" si="7"/>
-        <v>{id: 'White Chocolate (Белый шоколад)', name: 'White Chocolate (Белый шоколад)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="196" spans="1:11">
+        <v>{name: 'White Chocolate (Белый шоколад)' },</v>
+      </c>
+      <c r="L195" t="str">
+        <f>CONCATENATE($F$1,$G$1,C195,$H$1,C195,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12">
       <c r="A196" t="s">
         <v>407</v>
       </c>
       <c r="B196" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">'Wintergreen (Мятные кофеты)', </v>
+        <v>'Wintergreen (Мятные кофеты)'</v>
       </c>
       <c r="K196" t="str">
         <f t="shared" si="7"/>
-        <v>{id: 'Wintergreen (Мятные кофеты)', name: 'Wintergreen (Мятные кофеты)', isSelected: false },</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11">
+        <v>{name: 'Wintergreen (Мятные кофеты)' },</v>
+      </c>
+      <c r="L196" t="str">
+        <f>CONCATENATE($F$1,$G$1,C196,$H$1,C196,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12">
       <c r="A197" t="s">
         <v>219</v>
       </c>
       <c r="B197" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">'Yam (Ямс)', </v>
+        <v>'Yam (Ямс)'</v>
       </c>
       <c r="K197" t="str">
         <f t="shared" si="7"/>
-        <v>{id: 'Yam (Ямс)', name: 'Yam (Ямс)', isSelected: false },</v>
+        <v>{name: 'Yam (Ямс)' },</v>
+      </c>
+      <c r="L197" t="str">
+        <f>CONCATENATE($F$1,$G$1,C197,$H$1,C197,$I$1)</f>
+        <v>{id: name: isSelected: false</v>
       </c>
     </row>
   </sheetData>

</xml_diff>